<commit_message>
Update project + merge Audio player
</commit_message>
<xml_diff>
--- a/Document/OPPM2.xlsx
+++ b/Document/OPPM2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\CDW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\DACNPM\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D097BD0-F137-4763-BDE0-01D95604CD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB96450B-F626-4519-A94A-D89383D3ECDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,7 +385,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,13 +406,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,7 +724,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -775,9 +781,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -798,41 +801,78 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
@@ -843,59 +883,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -903,15 +938,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -947,23 +973,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -971,6 +989,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -980,82 +1016,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1065,6 +1077,21 @@
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -3137,8 +3164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25:F44"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19:V23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -3151,33 +3178,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="122"/>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="123"/>
-      <c r="R1" s="123"/>
-      <c r="S1" s="123"/>
-      <c r="T1" s="123"/>
-      <c r="U1" s="123"/>
-      <c r="V1" s="123"/>
-      <c r="W1" s="123"/>
-      <c r="X1" s="123"/>
-      <c r="Y1" s="123"/>
-      <c r="Z1" s="123"/>
-      <c r="AA1" s="123"/>
+      <c r="A1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+      <c r="Y1" s="42"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
       <c r="AB1" s="16"/>
       <c r="AC1" s="16"/>
       <c r="AD1" s="16"/>
@@ -3185,187 +3212,187 @@
       <c r="AF1" s="16"/>
     </row>
     <row r="2" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="122"/>
-      <c r="B2" s="60"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="35" t="s">
+      <c r="A2" s="41"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
-      <c r="R2" s="36"/>
-      <c r="S2" s="36"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="36"/>
-      <c r="V2" s="36"/>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="36"/>
-      <c r="Z2" s="36"/>
-      <c r="AA2" s="36"/>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="37"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+      <c r="R2" s="121"/>
+      <c r="S2" s="121"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="121"/>
+      <c r="V2" s="121"/>
+      <c r="W2" s="121"/>
+      <c r="X2" s="121"/>
+      <c r="Y2" s="121"/>
+      <c r="Z2" s="121"/>
+      <c r="AA2" s="121"/>
+      <c r="AB2" s="121"/>
+      <c r="AC2" s="122"/>
       <c r="AD2" s="16"/>
       <c r="AE2" s="16"/>
       <c r="AF2" s="16"/>
     </row>
     <row r="3" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="122"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="39"/>
-      <c r="Y3" s="39"/>
-      <c r="Z3" s="39"/>
-      <c r="AA3" s="39"/>
-      <c r="AB3" s="39"/>
-      <c r="AC3" s="40"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="110"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124"/>
+      <c r="N3" s="124"/>
+      <c r="O3" s="124"/>
+      <c r="P3" s="124"/>
+      <c r="Q3" s="124"/>
+      <c r="R3" s="124"/>
+      <c r="S3" s="124"/>
+      <c r="T3" s="124"/>
+      <c r="U3" s="124"/>
+      <c r="V3" s="124"/>
+      <c r="W3" s="124"/>
+      <c r="X3" s="124"/>
+      <c r="Y3" s="124"/>
+      <c r="Z3" s="124"/>
+      <c r="AA3" s="124"/>
+      <c r="AB3" s="124"/>
+      <c r="AC3" s="125"/>
       <c r="AD3" s="16"/>
       <c r="AE3" s="16"/>
       <c r="AF3" s="16"/>
     </row>
     <row r="4" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="122"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="39"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="39"/>
-      <c r="AC4" s="40"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
+      <c r="G4" s="123"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="124"/>
+      <c r="L4" s="124"/>
+      <c r="M4" s="124"/>
+      <c r="N4" s="124"/>
+      <c r="O4" s="124"/>
+      <c r="P4" s="124"/>
+      <c r="Q4" s="124"/>
+      <c r="R4" s="124"/>
+      <c r="S4" s="124"/>
+      <c r="T4" s="124"/>
+      <c r="U4" s="124"/>
+      <c r="V4" s="124"/>
+      <c r="W4" s="124"/>
+      <c r="X4" s="124"/>
+      <c r="Y4" s="124"/>
+      <c r="Z4" s="124"/>
+      <c r="AA4" s="124"/>
+      <c r="AB4" s="124"/>
+      <c r="AC4" s="125"/>
       <c r="AD4" s="16"/>
       <c r="AE4" s="16"/>
       <c r="AF4" s="16"/>
     </row>
     <row r="5" spans="1:32" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="122"/>
-      <c r="B5" s="64"/>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-      <c r="P5" s="42"/>
-      <c r="Q5" s="42"/>
-      <c r="R5" s="42"/>
-      <c r="S5" s="42"/>
-      <c r="T5" s="42"/>
-      <c r="U5" s="42"/>
-      <c r="V5" s="42"/>
-      <c r="W5" s="42"/>
-      <c r="X5" s="42"/>
-      <c r="Y5" s="42"/>
-      <c r="Z5" s="42"/>
-      <c r="AA5" s="42"/>
-      <c r="AB5" s="42"/>
-      <c r="AC5" s="43"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="113"/>
+      <c r="D5" s="113"/>
+      <c r="E5" s="113"/>
+      <c r="F5" s="113"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="127"/>
+      <c r="J5" s="127"/>
+      <c r="K5" s="127"/>
+      <c r="L5" s="127"/>
+      <c r="M5" s="127"/>
+      <c r="N5" s="127"/>
+      <c r="O5" s="127"/>
+      <c r="P5" s="127"/>
+      <c r="Q5" s="127"/>
+      <c r="R5" s="127"/>
+      <c r="S5" s="127"/>
+      <c r="T5" s="127"/>
+      <c r="U5" s="127"/>
+      <c r="V5" s="127"/>
+      <c r="W5" s="127"/>
+      <c r="X5" s="127"/>
+      <c r="Y5" s="127"/>
+      <c r="Z5" s="127"/>
+      <c r="AA5" s="127"/>
+      <c r="AB5" s="127"/>
+      <c r="AC5" s="128"/>
       <c r="AD5" s="16"/>
       <c r="AE5" s="16"/>
       <c r="AF5" s="16"/>
     </row>
     <row r="6" spans="1:32" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="122"/>
-      <c r="B6" s="44" t="s">
+      <c r="A6" s="41"/>
+      <c r="B6" s="104" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="97"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="107"/>
       <c r="G6" s="14"/>
-      <c r="H6" s="119" t="s">
+      <c r="H6" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="120"/>
-      <c r="J6" s="120"/>
-      <c r="K6" s="120"/>
-      <c r="L6" s="120"/>
-      <c r="M6" s="120"/>
-      <c r="N6" s="121"/>
-      <c r="O6" s="77" t="s">
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="39"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="78"/>
-      <c r="Q6" s="78"/>
-      <c r="R6" s="78"/>
-      <c r="S6" s="78"/>
-      <c r="T6" s="78"/>
-      <c r="U6" s="78"/>
-      <c r="V6" s="78"/>
-      <c r="W6" s="78"/>
-      <c r="X6" s="79"/>
-      <c r="Y6" s="44" t="s">
+      <c r="P6" s="90"/>
+      <c r="Q6" s="90"/>
+      <c r="R6" s="90"/>
+      <c r="S6" s="90"/>
+      <c r="T6" s="90"/>
+      <c r="U6" s="90"/>
+      <c r="V6" s="90"/>
+      <c r="W6" s="90"/>
+      <c r="X6" s="91"/>
+      <c r="Y6" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="Z6" s="45"/>
-      <c r="AA6" s="45"/>
-      <c r="AB6" s="45"/>
-      <c r="AC6" s="46"/>
+      <c r="Z6" s="105"/>
+      <c r="AA6" s="105"/>
+      <c r="AB6" s="105"/>
+      <c r="AC6" s="129"/>
       <c r="AD6" s="16"/>
       <c r="AE6" s="16"/>
       <c r="AF6" s="16"/>
     </row>
     <row r="7" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="122"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="20" t="s">
         <v>5</v>
       </c>
@@ -3384,22 +3411,22 @@
       <c r="G7" s="10">
         <v>1</v>
       </c>
-      <c r="H7" s="69" t="s">
+      <c r="H7" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="70"/>
-      <c r="O7" s="30" t="s">
+      <c r="I7" s="50"/>
+      <c r="J7" s="50"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="50"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="P7" s="31" t="s">
+      <c r="P7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="31" t="s">
+      <c r="Q7" s="30" t="s">
         <v>5</v>
       </c>
       <c r="R7" s="21"/>
@@ -3421,7 +3448,7 @@
       <c r="AF7" s="16"/>
     </row>
     <row r="8" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="122"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="23"/>
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
@@ -3430,22 +3457,22 @@
       <c r="G8" s="11">
         <v>2</v>
       </c>
-      <c r="H8" s="52" t="s">
+      <c r="H8" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="52"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="53"/>
-      <c r="O8" s="32" t="s">
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="P8" s="33" t="s">
+      <c r="P8" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="Q8" s="33" t="s">
+      <c r="Q8" s="32" t="s">
         <v>5</v>
       </c>
       <c r="R8" s="24"/>
@@ -3469,7 +3496,7 @@
       <c r="AF8" s="16"/>
     </row>
     <row r="9" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="122"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="23" t="s">
         <v>5</v>
       </c>
@@ -3482,41 +3509,41 @@
       <c r="G9" s="11">
         <v>3</v>
       </c>
-      <c r="H9" s="66" t="s">
+      <c r="H9" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="66"/>
-      <c r="L9" s="66"/>
-      <c r="M9" s="66"/>
-      <c r="N9" s="67"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="103"/>
+      <c r="L9" s="103"/>
+      <c r="M9" s="103"/>
+      <c r="N9" s="58"/>
       <c r="O9" s="23"/>
-      <c r="P9" s="33" t="s">
+      <c r="P9" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="Q9" s="33" t="s">
+      <c r="Q9" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="R9" s="33" t="s">
+      <c r="R9" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="S9" s="34" t="s">
+      <c r="S9" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="T9" s="34" t="s">
+      <c r="T9" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="U9" s="34" t="s">
+      <c r="U9" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="V9" s="24" t="s">
+      <c r="V9" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="W9" s="24" t="s">
+      <c r="W9" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="X9" s="25"/>
+      <c r="X9" s="138"/>
       <c r="Y9" s="11" t="s">
         <v>6</v>
       </c>
@@ -3537,7 +3564,7 @@
       <c r="AF9" s="16"/>
     </row>
     <row r="10" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="122"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
@@ -3546,29 +3573,29 @@
       <c r="G10" s="11">
         <v>4</v>
       </c>
-      <c r="H10" s="66" t="s">
+      <c r="H10" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="67"/>
+      <c r="I10" s="103"/>
+      <c r="J10" s="103"/>
+      <c r="K10" s="103"/>
+      <c r="L10" s="103"/>
+      <c r="M10" s="103"/>
+      <c r="N10" s="58"/>
       <c r="O10" s="23"/>
       <c r="P10" s="24"/>
       <c r="Q10" s="24"/>
-      <c r="R10" s="33" t="s">
+      <c r="R10" s="32" t="s">
         <v>5</v>
       </c>
       <c r="S10" s="24"/>
       <c r="T10" s="24"/>
-      <c r="U10" s="127" t="s">
+      <c r="U10" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="V10" s="24"/>
-      <c r="W10" s="24"/>
-      <c r="X10" s="25"/>
+      <c r="V10" s="33"/>
+      <c r="W10" s="33"/>
+      <c r="X10" s="138"/>
       <c r="Y10" s="11" t="s">
         <v>6</v>
       </c>
@@ -3581,7 +3608,7 @@
       <c r="AF10" s="16"/>
     </row>
     <row r="11" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="122"/>
+      <c r="A11" s="41"/>
       <c r="B11" s="23"/>
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
@@ -3590,33 +3617,33 @@
       <c r="G11" s="11">
         <v>5</v>
       </c>
-      <c r="H11" s="52" t="s">
+      <c r="H11" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="52"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="54"/>
       <c r="O11" s="23"/>
       <c r="P11" s="24"/>
       <c r="Q11" s="24"/>
-      <c r="R11" s="33" t="s">
+      <c r="R11" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="S11" s="34" t="s">
+      <c r="S11" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="T11" s="34" t="s">
+      <c r="T11" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="U11" s="127" t="s">
+      <c r="U11" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="25"/>
+      <c r="V11" s="33"/>
+      <c r="W11" s="33"/>
+      <c r="X11" s="138"/>
       <c r="Y11" s="11"/>
       <c r="Z11" s="12" t="s">
         <v>7</v>
@@ -3633,7 +3660,7 @@
       <c r="AF11" s="16"/>
     </row>
     <row r="12" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="122"/>
+      <c r="A12" s="41"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
@@ -3642,33 +3669,33 @@
       <c r="G12" s="11">
         <v>6</v>
       </c>
-      <c r="H12" s="52" t="s">
+      <c r="H12" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="53"/>
+      <c r="N12" s="54"/>
       <c r="O12" s="23"/>
       <c r="P12" s="24"/>
       <c r="Q12" s="24"/>
       <c r="R12" s="24"/>
-      <c r="S12" s="34" t="s">
+      <c r="S12" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="T12" s="34" t="s">
+      <c r="T12" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="U12" s="34" t="s">
+      <c r="U12" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="V12" s="24" t="s">
+      <c r="V12" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="W12" s="24"/>
-      <c r="X12" s="25"/>
+      <c r="W12" s="33"/>
+      <c r="X12" s="138"/>
       <c r="Y12" s="11" t="s">
         <v>6</v>
       </c>
@@ -3687,7 +3714,7 @@
       <c r="AF12" s="16"/>
     </row>
     <row r="13" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="122"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="23"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
@@ -3696,33 +3723,33 @@
       <c r="G13" s="11">
         <v>7</v>
       </c>
-      <c r="H13" s="68" t="s">
+      <c r="H13" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="68"/>
-      <c r="M13" s="68"/>
-      <c r="N13" s="68"/>
+      <c r="I13" s="102"/>
+      <c r="J13" s="102"/>
+      <c r="K13" s="102"/>
+      <c r="L13" s="102"/>
+      <c r="M13" s="102"/>
+      <c r="N13" s="102"/>
       <c r="O13" s="23"/>
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
       <c r="R13" s="24"/>
-      <c r="S13" s="34" t="s">
+      <c r="S13" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="T13" s="34" t="s">
+      <c r="T13" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="U13" s="34" t="s">
+      <c r="U13" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="V13" s="24" t="s">
+      <c r="V13" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="W13" s="24"/>
-      <c r="X13" s="25"/>
+      <c r="W13" s="33"/>
+      <c r="X13" s="138"/>
       <c r="Y13" s="11" t="s">
         <v>7</v>
       </c>
@@ -3739,7 +3766,7 @@
       <c r="AF13" s="16"/>
     </row>
     <row r="14" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="122"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
       <c r="D14" s="24" t="s">
@@ -3752,33 +3779,33 @@
       <c r="G14" s="11">
         <v>8</v>
       </c>
-      <c r="H14" s="68" t="s">
+      <c r="H14" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="68"/>
-      <c r="M14" s="68"/>
-      <c r="N14" s="68"/>
+      <c r="I14" s="102"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="102"/>
       <c r="O14" s="23"/>
       <c r="P14" s="24"/>
       <c r="Q14" s="24"/>
       <c r="R14" s="24"/>
       <c r="S14" s="24"/>
-      <c r="T14" s="127" t="s">
+      <c r="T14" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="U14" s="127" t="s">
+      <c r="U14" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="V14" s="24" t="s">
+      <c r="V14" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="W14" s="24" t="s">
+      <c r="W14" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="X14" s="25"/>
+      <c r="X14" s="138"/>
       <c r="Y14" s="11" t="s">
         <v>6</v>
       </c>
@@ -3797,7 +3824,7 @@
       <c r="AF14" s="16"/>
     </row>
     <row r="15" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="122"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="23"/>
       <c r="C15" s="24"/>
       <c r="D15" s="24" t="s">
@@ -3810,33 +3837,33 @@
       <c r="G15" s="11">
         <v>9</v>
       </c>
-      <c r="H15" s="68" t="s">
+      <c r="H15" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="68"/>
-      <c r="N15" s="68"/>
+      <c r="I15" s="102"/>
+      <c r="J15" s="102"/>
+      <c r="K15" s="102"/>
+      <c r="L15" s="102"/>
+      <c r="M15" s="102"/>
+      <c r="N15" s="102"/>
       <c r="O15" s="23"/>
       <c r="P15" s="24"/>
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
       <c r="S15" s="24"/>
-      <c r="T15" s="128" t="s">
+      <c r="T15" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="U15" s="34" t="s">
+      <c r="U15" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="V15" s="24" t="s">
+      <c r="V15" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="W15" s="24" t="s">
+      <c r="W15" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="X15" s="25"/>
+      <c r="X15" s="138"/>
       <c r="Y15" s="11"/>
       <c r="Z15" s="13" t="s">
         <v>6</v>
@@ -3849,7 +3876,7 @@
       <c r="AF15" s="16"/>
     </row>
     <row r="16" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="122"/>
+      <c r="A16" s="41"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24"/>
       <c r="D16" s="24"/>
@@ -3860,35 +3887,35 @@
       <c r="G16" s="11">
         <v>10</v>
       </c>
-      <c r="H16" s="68" t="s">
+      <c r="H16" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="I16" s="68"/>
-      <c r="J16" s="68"/>
-      <c r="K16" s="68"/>
-      <c r="L16" s="68"/>
-      <c r="M16" s="68"/>
-      <c r="N16" s="68"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="102"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="102"/>
+      <c r="N16" s="102"/>
       <c r="O16" s="23"/>
       <c r="P16" s="24"/>
       <c r="Q16" s="24"/>
       <c r="R16" s="24"/>
-      <c r="S16" s="128" t="s">
+      <c r="S16" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="T16" s="34" t="s">
+      <c r="T16" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="U16" s="129" t="s">
+      <c r="U16" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="V16" s="26" t="s">
+      <c r="V16" s="139" t="s">
         <v>5</v>
       </c>
-      <c r="W16" s="24" t="s">
+      <c r="W16" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="X16" s="25"/>
+      <c r="X16" s="138"/>
       <c r="Y16" s="11" t="s">
         <v>6</v>
       </c>
@@ -3909,7 +3936,7 @@
       <c r="AF16" s="16"/>
     </row>
     <row r="17" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="122"/>
+      <c r="A17" s="41"/>
       <c r="B17" s="23"/>
       <c r="C17" s="24"/>
       <c r="D17" s="24"/>
@@ -3920,15 +3947,15 @@
       <c r="G17" s="11">
         <v>11</v>
       </c>
-      <c r="H17" s="68" t="s">
+      <c r="H17" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="68"/>
-      <c r="J17" s="68"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="68"/>
-      <c r="M17" s="68"/>
-      <c r="N17" s="68"/>
+      <c r="I17" s="102"/>
+      <c r="J17" s="102"/>
+      <c r="K17" s="102"/>
+      <c r="L17" s="102"/>
+      <c r="M17" s="102"/>
+      <c r="N17" s="102"/>
       <c r="O17" s="23"/>
       <c r="P17" s="24"/>
       <c r="Q17" s="24"/>
@@ -3936,9 +3963,9 @@
       <c r="S17" s="24"/>
       <c r="T17" s="24"/>
       <c r="U17" s="24"/>
-      <c r="V17" s="24"/>
-      <c r="W17" s="24"/>
-      <c r="X17" s="25" t="s">
+      <c r="V17" s="33"/>
+      <c r="W17" s="33"/>
+      <c r="X17" s="138" t="s">
         <v>5</v>
       </c>
       <c r="Y17" s="11"/>
@@ -3955,20 +3982,20 @@
       <c r="AF17" s="16"/>
     </row>
     <row r="18" spans="1:32" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="122"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
       <c r="E18" s="24"/>
       <c r="F18" s="25"/>
       <c r="G18" s="11"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
-      <c r="J18" s="52"/>
-      <c r="K18" s="52"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="52"/>
-      <c r="N18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
+      <c r="M18" s="53"/>
+      <c r="N18" s="54"/>
       <c r="O18" s="23"/>
       <c r="P18" s="24"/>
       <c r="Q18" s="24"/>
@@ -3981,7 +4008,7 @@
       <c r="X18" s="25"/>
       <c r="Y18" s="11"/>
       <c r="Z18" s="12"/>
-      <c r="AA18" s="27"/>
+      <c r="AA18" s="26"/>
       <c r="AB18" s="18"/>
       <c r="AC18" s="19"/>
       <c r="AD18" s="16"/>
@@ -3989,63 +4016,63 @@
       <c r="AF18" s="16"/>
     </row>
     <row r="19" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="122"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="3"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="86"/>
-      <c r="I19" s="86"/>
-      <c r="J19" s="86"/>
-      <c r="K19" s="86"/>
-      <c r="L19" s="86"/>
-      <c r="M19" s="86"/>
-      <c r="N19" s="87"/>
-      <c r="O19" s="93">
+      <c r="H19" s="98"/>
+      <c r="I19" s="98"/>
+      <c r="J19" s="98"/>
+      <c r="K19" s="98"/>
+      <c r="L19" s="98"/>
+      <c r="M19" s="98"/>
+      <c r="N19" s="99"/>
+      <c r="O19" s="43">
         <v>44641</v>
       </c>
-      <c r="P19" s="93">
+      <c r="P19" s="43">
         <v>44648</v>
       </c>
-      <c r="Q19" s="93">
+      <c r="Q19" s="43">
         <v>44655</v>
       </c>
-      <c r="R19" s="130">
+      <c r="R19" s="46">
         <v>44662</v>
       </c>
-      <c r="S19" s="93" t="s">
+      <c r="S19" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="T19" s="93" t="s">
+      <c r="T19" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="U19" s="133">
+      <c r="U19" s="132">
         <v>44683</v>
       </c>
-      <c r="V19" s="130">
+      <c r="V19" s="140">
         <v>44690</v>
       </c>
-      <c r="W19" s="93" t="s">
+      <c r="W19" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="X19" s="130" t="s">
+      <c r="X19" s="135" t="s">
         <v>39</v>
       </c>
-      <c r="Y19" s="90" t="s">
+      <c r="Y19" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="Z19" s="90" t="s">
+      <c r="Z19" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="AA19" s="47" t="s">
+      <c r="AA19" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="AB19" s="47" t="s">
+      <c r="AB19" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="AC19" s="47" t="s">
+      <c r="AC19" s="65" t="s">
         <v>32</v>
       </c>
       <c r="AD19" s="16"/>
@@ -4053,158 +4080,158 @@
       <c r="AF19" s="16"/>
     </row>
     <row r="20" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="122"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="4"/>
       <c r="C20" s="7"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
       <c r="F20" s="6"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="88"/>
-      <c r="L20" s="88"/>
-      <c r="M20" s="88"/>
-      <c r="N20" s="89"/>
-      <c r="O20" s="94"/>
-      <c r="P20" s="94"/>
-      <c r="Q20" s="94"/>
-      <c r="R20" s="131"/>
-      <c r="S20" s="94"/>
-      <c r="T20" s="94"/>
-      <c r="U20" s="134"/>
-      <c r="V20" s="131"/>
-      <c r="W20" s="94"/>
-      <c r="X20" s="131"/>
-      <c r="Y20" s="91"/>
-      <c r="Z20" s="91"/>
-      <c r="AA20" s="48"/>
-      <c r="AB20" s="48"/>
-      <c r="AC20" s="48"/>
+      <c r="H20" s="100"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="100"/>
+      <c r="K20" s="100"/>
+      <c r="L20" s="100"/>
+      <c r="M20" s="100"/>
+      <c r="N20" s="101"/>
+      <c r="O20" s="44"/>
+      <c r="P20" s="44"/>
+      <c r="Q20" s="44"/>
+      <c r="R20" s="47"/>
+      <c r="S20" s="44"/>
+      <c r="T20" s="44"/>
+      <c r="U20" s="133"/>
+      <c r="V20" s="141"/>
+      <c r="W20" s="44"/>
+      <c r="X20" s="136"/>
+      <c r="Y20" s="63"/>
+      <c r="Z20" s="63"/>
+      <c r="AA20" s="66"/>
+      <c r="AB20" s="66"/>
+      <c r="AC20" s="66"/>
       <c r="AD20" s="16"/>
       <c r="AE20" s="16"/>
       <c r="AF20" s="16"/>
     </row>
     <row r="21" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="122"/>
+      <c r="A21" s="41"/>
       <c r="B21" s="4"/>
       <c r="C21" s="7"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
       <c r="F21" s="6"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="88"/>
-      <c r="I21" s="88"/>
-      <c r="J21" s="88"/>
-      <c r="K21" s="88"/>
-      <c r="L21" s="88"/>
-      <c r="M21" s="88"/>
-      <c r="N21" s="89"/>
-      <c r="O21" s="94"/>
-      <c r="P21" s="94"/>
-      <c r="Q21" s="94"/>
-      <c r="R21" s="131"/>
-      <c r="S21" s="94"/>
-      <c r="T21" s="94"/>
-      <c r="U21" s="134"/>
-      <c r="V21" s="131"/>
-      <c r="W21" s="94"/>
-      <c r="X21" s="131"/>
-      <c r="Y21" s="91"/>
-      <c r="Z21" s="91"/>
-      <c r="AA21" s="48"/>
-      <c r="AB21" s="48"/>
-      <c r="AC21" s="48"/>
+      <c r="H21" s="100"/>
+      <c r="I21" s="100"/>
+      <c r="J21" s="100"/>
+      <c r="K21" s="100"/>
+      <c r="L21" s="100"/>
+      <c r="M21" s="100"/>
+      <c r="N21" s="101"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="44"/>
+      <c r="Q21" s="44"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="44"/>
+      <c r="T21" s="44"/>
+      <c r="U21" s="133"/>
+      <c r="V21" s="141"/>
+      <c r="W21" s="44"/>
+      <c r="X21" s="136"/>
+      <c r="Y21" s="63"/>
+      <c r="Z21" s="63"/>
+      <c r="AA21" s="66"/>
+      <c r="AB21" s="66"/>
+      <c r="AC21" s="66"/>
       <c r="AD21" s="16"/>
       <c r="AE21" s="16"/>
       <c r="AF21" s="16"/>
     </row>
     <row r="22" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="122"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="4"/>
       <c r="C22" s="7"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="6"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="88"/>
-      <c r="I22" s="88"/>
-      <c r="J22" s="88"/>
-      <c r="K22" s="88"/>
-      <c r="L22" s="88"/>
-      <c r="M22" s="88"/>
-      <c r="N22" s="89"/>
-      <c r="O22" s="94"/>
-      <c r="P22" s="94"/>
-      <c r="Q22" s="94"/>
-      <c r="R22" s="131"/>
-      <c r="S22" s="94"/>
-      <c r="T22" s="94"/>
-      <c r="U22" s="134"/>
-      <c r="V22" s="131"/>
-      <c r="W22" s="94"/>
-      <c r="X22" s="131"/>
-      <c r="Y22" s="91"/>
-      <c r="Z22" s="91"/>
-      <c r="AA22" s="48"/>
-      <c r="AB22" s="48"/>
-      <c r="AC22" s="48"/>
+      <c r="H22" s="100"/>
+      <c r="I22" s="100"/>
+      <c r="J22" s="100"/>
+      <c r="K22" s="100"/>
+      <c r="L22" s="100"/>
+      <c r="M22" s="100"/>
+      <c r="N22" s="101"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="44"/>
+      <c r="Q22" s="44"/>
+      <c r="R22" s="47"/>
+      <c r="S22" s="44"/>
+      <c r="T22" s="44"/>
+      <c r="U22" s="133"/>
+      <c r="V22" s="141"/>
+      <c r="W22" s="44"/>
+      <c r="X22" s="136"/>
+      <c r="Y22" s="63"/>
+      <c r="Z22" s="63"/>
+      <c r="AA22" s="66"/>
+      <c r="AB22" s="66"/>
+      <c r="AC22" s="66"/>
       <c r="AD22" s="16"/>
       <c r="AE22" s="16"/>
       <c r="AF22" s="16"/>
     </row>
     <row r="23" spans="1:32" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="122"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="4"/>
       <c r="C23" s="7"/>
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="6"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="78"/>
-      <c r="L23" s="78"/>
-      <c r="M23" s="78"/>
-      <c r="N23" s="79"/>
-      <c r="O23" s="95"/>
-      <c r="P23" s="95"/>
-      <c r="Q23" s="95"/>
-      <c r="R23" s="132"/>
-      <c r="S23" s="95"/>
-      <c r="T23" s="95"/>
-      <c r="U23" s="135"/>
-      <c r="V23" s="132"/>
-      <c r="W23" s="95"/>
-      <c r="X23" s="132"/>
-      <c r="Y23" s="92"/>
-      <c r="Z23" s="92"/>
-      <c r="AA23" s="49"/>
-      <c r="AB23" s="49"/>
-      <c r="AC23" s="49"/>
+      <c r="H23" s="90"/>
+      <c r="I23" s="90"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="90"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="90"/>
+      <c r="N23" s="91"/>
+      <c r="O23" s="45"/>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="45"/>
+      <c r="R23" s="48"/>
+      <c r="S23" s="45"/>
+      <c r="T23" s="45"/>
+      <c r="U23" s="134"/>
+      <c r="V23" s="142"/>
+      <c r="W23" s="45"/>
+      <c r="X23" s="137"/>
+      <c r="Y23" s="64"/>
+      <c r="Z23" s="64"/>
+      <c r="AA23" s="67"/>
+      <c r="AB23" s="67"/>
+      <c r="AC23" s="67"/>
       <c r="AD23" s="16"/>
       <c r="AE23" s="16"/>
       <c r="AF23" s="16"/>
     </row>
     <row r="24" spans="1:32" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="122"/>
-      <c r="B24" s="80"/>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="82"/>
-      <c r="G24" s="83" t="s">
+      <c r="A24" s="41"/>
+      <c r="B24" s="92"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="93"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="H24" s="84"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="84"/>
-      <c r="K24" s="84"/>
-      <c r="L24" s="84"/>
-      <c r="M24" s="84"/>
-      <c r="N24" s="85"/>
+      <c r="H24" s="96"/>
+      <c r="I24" s="96"/>
+      <c r="J24" s="96"/>
+      <c r="K24" s="96"/>
+      <c r="L24" s="96"/>
+      <c r="M24" s="96"/>
+      <c r="N24" s="97"/>
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
@@ -4215,53 +4242,53 @@
       <c r="V24" s="8"/>
       <c r="W24" s="8"/>
       <c r="X24" s="9"/>
-      <c r="Y24" s="28"/>
-      <c r="Z24" s="29"/>
-      <c r="AA24" s="50"/>
-      <c r="AB24" s="50"/>
-      <c r="AC24" s="51"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="28"/>
+      <c r="AA24" s="130"/>
+      <c r="AB24" s="130"/>
+      <c r="AC24" s="131"/>
       <c r="AD24" s="16"/>
       <c r="AE24" s="16"/>
       <c r="AF24" s="16"/>
     </row>
     <row r="25" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="122"/>
-      <c r="B25" s="47" t="s">
+      <c r="A25" s="41"/>
+      <c r="B25" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="47" t="s">
+      <c r="D25" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="F25" s="47" t="s">
+      <c r="F25" s="65" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="124"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="69"/>
-      <c r="N25" s="70"/>
-      <c r="O25" s="116"/>
-      <c r="P25" s="117"/>
-      <c r="Q25" s="117"/>
-      <c r="R25" s="117"/>
-      <c r="S25" s="117"/>
-      <c r="T25" s="117"/>
-      <c r="U25" s="117"/>
-      <c r="V25" s="117"/>
-      <c r="W25" s="117"/>
-      <c r="X25" s="117"/>
-      <c r="Y25" s="117"/>
-      <c r="Z25" s="117"/>
-      <c r="AA25" s="112"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
+      <c r="J25" s="50"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="51"/>
+      <c r="O25" s="84"/>
+      <c r="P25" s="85"/>
+      <c r="Q25" s="85"/>
+      <c r="R25" s="85"/>
+      <c r="S25" s="85"/>
+      <c r="T25" s="85"/>
+      <c r="U25" s="85"/>
+      <c r="V25" s="85"/>
+      <c r="W25" s="85"/>
+      <c r="X25" s="85"/>
+      <c r="Y25" s="85"/>
+      <c r="Z25" s="85"/>
+      <c r="AA25" s="78"/>
       <c r="AB25" s="16"/>
       <c r="AC25" s="16"/>
       <c r="AD25" s="16"/>
@@ -4269,39 +4296,39 @@
       <c r="AF25" s="16"/>
     </row>
     <row r="26" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="122"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="48"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="125"/>
-      <c r="H26" s="52"/>
-      <c r="I26" s="52"/>
-      <c r="J26" s="52"/>
-      <c r="K26" s="52"/>
-      <c r="L26" s="52"/>
-      <c r="M26" s="52"/>
-      <c r="N26" s="52"/>
-      <c r="O26" s="57"/>
-      <c r="P26" s="54"/>
-      <c r="Q26" s="54"/>
-      <c r="R26" s="54"/>
-      <c r="S26" s="54"/>
-      <c r="T26" s="54"/>
-      <c r="U26" s="54"/>
-      <c r="V26" s="54" t="s">
+      <c r="A26" s="41"/>
+      <c r="B26" s="66"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="117"/>
+      <c r="P26" s="77"/>
+      <c r="Q26" s="77"/>
+      <c r="R26" s="77"/>
+      <c r="S26" s="77"/>
+      <c r="T26" s="77"/>
+      <c r="U26" s="77"/>
+      <c r="V26" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="W26" s="54"/>
-      <c r="X26" s="54" t="s">
+      <c r="W26" s="77"/>
+      <c r="X26" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="Y26" s="54"/>
-      <c r="Z26" s="54" t="s">
+      <c r="Y26" s="77"/>
+      <c r="Z26" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="AA26" s="112"/>
+      <c r="AA26" s="78"/>
       <c r="AB26" s="16"/>
       <c r="AC26" s="16"/>
       <c r="AD26" s="16"/>
@@ -4309,41 +4336,41 @@
       <c r="AF26" s="16"/>
     </row>
     <row r="27" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="122"/>
-      <c r="B27" s="48"/>
-      <c r="C27" s="48"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="125"/>
-      <c r="H27" s="52"/>
-      <c r="I27" s="52"/>
-      <c r="J27" s="52"/>
-      <c r="K27" s="52"/>
-      <c r="L27" s="52"/>
-      <c r="M27" s="52"/>
-      <c r="N27" s="52"/>
-      <c r="O27" s="58" t="s">
+      <c r="A27" s="41"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="66"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="66"/>
+      <c r="G27" s="52"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="53"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
+      <c r="O27" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="P27" s="59"/>
-      <c r="Q27" s="59"/>
-      <c r="R27" s="59"/>
-      <c r="S27" s="59"/>
-      <c r="T27" s="59"/>
-      <c r="U27" s="59"/>
-      <c r="V27" s="54">
+      <c r="P27" s="119"/>
+      <c r="Q27" s="119"/>
+      <c r="R27" s="119"/>
+      <c r="S27" s="119"/>
+      <c r="T27" s="119"/>
+      <c r="U27" s="119"/>
+      <c r="V27" s="77">
         <v>0</v>
       </c>
-      <c r="W27" s="54"/>
-      <c r="X27" s="54">
+      <c r="W27" s="77"/>
+      <c r="X27" s="77">
         <v>0</v>
       </c>
-      <c r="Y27" s="54"/>
-      <c r="Z27" s="55">
+      <c r="Y27" s="77"/>
+      <c r="Z27" s="79">
         <v>0</v>
       </c>
-      <c r="AA27" s="56"/>
+      <c r="AA27" s="80"/>
       <c r="AB27" s="16"/>
       <c r="AC27" s="16"/>
       <c r="AD27" s="16"/>
@@ -4351,42 +4378,42 @@
       <c r="AF27" s="16"/>
     </row>
     <row r="28" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="122"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="125"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="52"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="52"/>
-      <c r="M28" s="52"/>
-      <c r="N28" s="52"/>
-      <c r="O28" s="58" t="s">
+      <c r="A28" s="41"/>
+      <c r="B28" s="66"/>
+      <c r="C28" s="66"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="66"/>
+      <c r="F28" s="66"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
+      <c r="M28" s="53"/>
+      <c r="N28" s="53"/>
+      <c r="O28" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="P28" s="59"/>
-      <c r="Q28" s="59"/>
-      <c r="R28" s="59"/>
-      <c r="S28" s="59"/>
-      <c r="T28" s="59"/>
-      <c r="U28" s="59"/>
-      <c r="V28" s="54">
+      <c r="P28" s="119"/>
+      <c r="Q28" s="119"/>
+      <c r="R28" s="119"/>
+      <c r="S28" s="119"/>
+      <c r="T28" s="119"/>
+      <c r="U28" s="119"/>
+      <c r="V28" s="77">
         <v>0</v>
       </c>
-      <c r="W28" s="54"/>
-      <c r="X28" s="54">
+      <c r="W28" s="77"/>
+      <c r="X28" s="77">
         <v>0</v>
       </c>
-      <c r="Y28" s="54"/>
-      <c r="Z28" s="55">
+      <c r="Y28" s="77"/>
+      <c r="Z28" s="79">
         <f>-O291</f>
         <v>0</v>
       </c>
-      <c r="AA28" s="56"/>
+      <c r="AA28" s="80"/>
       <c r="AB28" s="16"/>
       <c r="AC28" s="16"/>
       <c r="AD28" s="16"/>
@@ -4394,41 +4421,41 @@
       <c r="AF28" s="16"/>
     </row>
     <row r="29" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="122"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
-      <c r="G29" s="125"/>
-      <c r="H29" s="52"/>
-      <c r="I29" s="52"/>
-      <c r="J29" s="52"/>
-      <c r="K29" s="52"/>
-      <c r="L29" s="52"/>
-      <c r="M29" s="52"/>
-      <c r="N29" s="52"/>
-      <c r="O29" s="58" t="s">
+      <c r="A29" s="41"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="66"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
+      <c r="M29" s="53"/>
+      <c r="N29" s="53"/>
+      <c r="O29" s="118" t="s">
         <v>13</v>
       </c>
-      <c r="P29" s="59"/>
-      <c r="Q29" s="59"/>
-      <c r="R29" s="59"/>
-      <c r="S29" s="59"/>
-      <c r="T29" s="59"/>
-      <c r="U29" s="59"/>
-      <c r="V29" s="54">
+      <c r="P29" s="119"/>
+      <c r="Q29" s="119"/>
+      <c r="R29" s="119"/>
+      <c r="S29" s="119"/>
+      <c r="T29" s="119"/>
+      <c r="U29" s="119"/>
+      <c r="V29" s="77">
         <v>0</v>
       </c>
-      <c r="W29" s="54"/>
-      <c r="X29" s="54">
+      <c r="W29" s="77"/>
+      <c r="X29" s="77">
         <v>0</v>
       </c>
-      <c r="Y29" s="54"/>
-      <c r="Z29" s="55">
+      <c r="Y29" s="77"/>
+      <c r="Z29" s="79">
         <v>0</v>
       </c>
-      <c r="AA29" s="56"/>
+      <c r="AA29" s="80"/>
       <c r="AB29" s="16"/>
       <c r="AC29" s="16"/>
       <c r="AD29" s="16"/>
@@ -4436,33 +4463,33 @@
       <c r="AF29" s="16"/>
     </row>
     <row r="30" spans="1:32" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="122"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="48"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="125"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
-      <c r="K30" s="52"/>
-      <c r="L30" s="52"/>
-      <c r="M30" s="52"/>
-      <c r="N30" s="53"/>
-      <c r="O30" s="113"/>
-      <c r="P30" s="114"/>
-      <c r="Q30" s="114"/>
-      <c r="R30" s="114"/>
-      <c r="S30" s="114"/>
-      <c r="T30" s="114"/>
-      <c r="U30" s="114"/>
-      <c r="V30" s="114"/>
-      <c r="W30" s="114"/>
-      <c r="X30" s="114"/>
-      <c r="Y30" s="114"/>
-      <c r="Z30" s="114"/>
-      <c r="AA30" s="115"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="53"/>
+      <c r="M30" s="53"/>
+      <c r="N30" s="54"/>
+      <c r="O30" s="81"/>
+      <c r="P30" s="82"/>
+      <c r="Q30" s="82"/>
+      <c r="R30" s="82"/>
+      <c r="S30" s="82"/>
+      <c r="T30" s="82"/>
+      <c r="U30" s="82"/>
+      <c r="V30" s="82"/>
+      <c r="W30" s="82"/>
+      <c r="X30" s="82"/>
+      <c r="Y30" s="82"/>
+      <c r="Z30" s="82"/>
+      <c r="AA30" s="83"/>
       <c r="AB30" s="16"/>
       <c r="AC30" s="16"/>
       <c r="AD30" s="16"/>
@@ -4470,35 +4497,35 @@
       <c r="AF30" s="16"/>
     </row>
     <row r="31" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="122"/>
-      <c r="B31" s="48"/>
-      <c r="C31" s="48"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
-      <c r="G31" s="125"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
-      <c r="K31" s="52"/>
-      <c r="L31" s="52"/>
-      <c r="M31" s="52"/>
-      <c r="N31" s="53"/>
-      <c r="O31" s="71" t="s">
+      <c r="A31" s="41"/>
+      <c r="B31" s="66"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="66"/>
+      <c r="F31" s="66"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="53"/>
+      <c r="M31" s="53"/>
+      <c r="N31" s="54"/>
+      <c r="O31" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="P31" s="72"/>
-      <c r="Q31" s="72"/>
-      <c r="R31" s="72"/>
-      <c r="S31" s="72"/>
-      <c r="T31" s="72"/>
-      <c r="U31" s="72"/>
-      <c r="V31" s="72"/>
-      <c r="W31" s="72"/>
-      <c r="X31" s="72"/>
-      <c r="Y31" s="72"/>
-      <c r="Z31" s="72"/>
-      <c r="AA31" s="73"/>
+      <c r="P31" s="87"/>
+      <c r="Q31" s="87"/>
+      <c r="R31" s="87"/>
+      <c r="S31" s="87"/>
+      <c r="T31" s="87"/>
+      <c r="U31" s="87"/>
+      <c r="V31" s="87"/>
+      <c r="W31" s="87"/>
+      <c r="X31" s="87"/>
+      <c r="Y31" s="87"/>
+      <c r="Z31" s="87"/>
+      <c r="AA31" s="88"/>
       <c r="AB31" s="16"/>
       <c r="AC31" s="16"/>
       <c r="AD31" s="16"/>
@@ -4506,33 +4533,33 @@
       <c r="AF31" s="16"/>
     </row>
     <row r="32" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="122"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
-      <c r="G32" s="125"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="52"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="52"/>
-      <c r="M32" s="52"/>
-      <c r="N32" s="53"/>
-      <c r="O32" s="74"/>
-      <c r="P32" s="75"/>
-      <c r="Q32" s="75"/>
-      <c r="R32" s="75"/>
-      <c r="S32" s="75"/>
-      <c r="T32" s="75"/>
-      <c r="U32" s="75"/>
-      <c r="V32" s="75"/>
-      <c r="W32" s="75"/>
-      <c r="X32" s="75"/>
-      <c r="Y32" s="75"/>
-      <c r="Z32" s="75"/>
-      <c r="AA32" s="76"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="53"/>
+      <c r="M32" s="53"/>
+      <c r="N32" s="54"/>
+      <c r="O32" s="68"/>
+      <c r="P32" s="69"/>
+      <c r="Q32" s="69"/>
+      <c r="R32" s="69"/>
+      <c r="S32" s="69"/>
+      <c r="T32" s="69"/>
+      <c r="U32" s="69"/>
+      <c r="V32" s="69"/>
+      <c r="W32" s="69"/>
+      <c r="X32" s="69"/>
+      <c r="Y32" s="69"/>
+      <c r="Z32" s="69"/>
+      <c r="AA32" s="70"/>
       <c r="AB32" s="16"/>
       <c r="AC32" s="16"/>
       <c r="AD32" s="16"/>
@@ -4540,35 +4567,35 @@
       <c r="AF32" s="16"/>
     </row>
     <row r="33" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="122"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="125"/>
-      <c r="H33" s="52"/>
-      <c r="I33" s="52"/>
-      <c r="J33" s="52"/>
-      <c r="K33" s="52"/>
-      <c r="L33" s="52"/>
-      <c r="M33" s="52"/>
-      <c r="N33" s="53"/>
-      <c r="O33" s="74" t="s">
+      <c r="A33" s="41"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="66"/>
+      <c r="G33" s="52"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="53"/>
+      <c r="M33" s="53"/>
+      <c r="N33" s="54"/>
+      <c r="O33" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="P33" s="75"/>
-      <c r="Q33" s="75"/>
-      <c r="R33" s="75"/>
-      <c r="S33" s="75"/>
-      <c r="T33" s="75"/>
-      <c r="U33" s="75"/>
-      <c r="V33" s="75"/>
-      <c r="W33" s="75"/>
-      <c r="X33" s="75"/>
-      <c r="Y33" s="75"/>
-      <c r="Z33" s="75"/>
-      <c r="AA33" s="76"/>
+      <c r="P33" s="69"/>
+      <c r="Q33" s="69"/>
+      <c r="R33" s="69"/>
+      <c r="S33" s="69"/>
+      <c r="T33" s="69"/>
+      <c r="U33" s="69"/>
+      <c r="V33" s="69"/>
+      <c r="W33" s="69"/>
+      <c r="X33" s="69"/>
+      <c r="Y33" s="69"/>
+      <c r="Z33" s="69"/>
+      <c r="AA33" s="70"/>
       <c r="AB33" s="16"/>
       <c r="AC33" s="16"/>
       <c r="AD33" s="16"/>
@@ -4576,33 +4603,33 @@
       <c r="AF33" s="16"/>
     </row>
     <row r="34" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="122"/>
-      <c r="B34" s="48"/>
-      <c r="C34" s="48"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="125"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
-      <c r="M34" s="52"/>
-      <c r="N34" s="53"/>
-      <c r="O34" s="74"/>
-      <c r="P34" s="75"/>
-      <c r="Q34" s="75"/>
-      <c r="R34" s="75"/>
-      <c r="S34" s="75"/>
-      <c r="T34" s="75"/>
-      <c r="U34" s="75"/>
-      <c r="V34" s="75"/>
-      <c r="W34" s="75"/>
-      <c r="X34" s="75"/>
-      <c r="Y34" s="75"/>
-      <c r="Z34" s="75"/>
-      <c r="AA34" s="76"/>
+      <c r="A34" s="41"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="66"/>
+      <c r="D34" s="66"/>
+      <c r="E34" s="66"/>
+      <c r="F34" s="66"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="53"/>
+      <c r="L34" s="53"/>
+      <c r="M34" s="53"/>
+      <c r="N34" s="54"/>
+      <c r="O34" s="68"/>
+      <c r="P34" s="69"/>
+      <c r="Q34" s="69"/>
+      <c r="R34" s="69"/>
+      <c r="S34" s="69"/>
+      <c r="T34" s="69"/>
+      <c r="U34" s="69"/>
+      <c r="V34" s="69"/>
+      <c r="W34" s="69"/>
+      <c r="X34" s="69"/>
+      <c r="Y34" s="69"/>
+      <c r="Z34" s="69"/>
+      <c r="AA34" s="70"/>
       <c r="AB34" s="16"/>
       <c r="AC34" s="16"/>
       <c r="AD34" s="16"/>
@@ -4610,35 +4637,35 @@
       <c r="AF34" s="16"/>
     </row>
     <row r="35" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="122"/>
-      <c r="B35" s="48"/>
-      <c r="C35" s="48"/>
-      <c r="D35" s="48"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="125"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="52"/>
-      <c r="N35" s="53"/>
-      <c r="O35" s="106" t="s">
+      <c r="A35" s="41"/>
+      <c r="B35" s="66"/>
+      <c r="C35" s="66"/>
+      <c r="D35" s="66"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="66"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="53"/>
+      <c r="I35" s="53"/>
+      <c r="J35" s="53"/>
+      <c r="K35" s="53"/>
+      <c r="L35" s="53"/>
+      <c r="M35" s="53"/>
+      <c r="N35" s="54"/>
+      <c r="O35" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="P35" s="107"/>
-      <c r="Q35" s="107"/>
-      <c r="R35" s="107"/>
-      <c r="S35" s="107"/>
-      <c r="T35" s="107"/>
-      <c r="U35" s="107"/>
-      <c r="V35" s="107"/>
-      <c r="W35" s="107"/>
-      <c r="X35" s="107"/>
-      <c r="Y35" s="107"/>
-      <c r="Z35" s="107"/>
-      <c r="AA35" s="108"/>
+      <c r="P35" s="72"/>
+      <c r="Q35" s="72"/>
+      <c r="R35" s="72"/>
+      <c r="S35" s="72"/>
+      <c r="T35" s="72"/>
+      <c r="U35" s="72"/>
+      <c r="V35" s="72"/>
+      <c r="W35" s="72"/>
+      <c r="X35" s="72"/>
+      <c r="Y35" s="72"/>
+      <c r="Z35" s="72"/>
+      <c r="AA35" s="73"/>
       <c r="AB35" s="16"/>
       <c r="AC35" s="16"/>
       <c r="AD35" s="16"/>
@@ -4646,33 +4673,33 @@
       <c r="AF35" s="16"/>
     </row>
     <row r="36" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="122"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="48"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
-      <c r="G36" s="125"/>
-      <c r="H36" s="52"/>
-      <c r="I36" s="52"/>
-      <c r="J36" s="52"/>
-      <c r="K36" s="52"/>
-      <c r="L36" s="52"/>
-      <c r="M36" s="52"/>
-      <c r="N36" s="53"/>
-      <c r="O36" s="106"/>
-      <c r="P36" s="107"/>
-      <c r="Q36" s="107"/>
-      <c r="R36" s="107"/>
-      <c r="S36" s="107"/>
-      <c r="T36" s="107"/>
-      <c r="U36" s="107"/>
-      <c r="V36" s="107"/>
-      <c r="W36" s="107"/>
-      <c r="X36" s="107"/>
-      <c r="Y36" s="107"/>
-      <c r="Z36" s="107"/>
-      <c r="AA36" s="108"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="66"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="53"/>
+      <c r="K36" s="53"/>
+      <c r="L36" s="53"/>
+      <c r="M36" s="53"/>
+      <c r="N36" s="54"/>
+      <c r="O36" s="71"/>
+      <c r="P36" s="72"/>
+      <c r="Q36" s="72"/>
+      <c r="R36" s="72"/>
+      <c r="S36" s="72"/>
+      <c r="T36" s="72"/>
+      <c r="U36" s="72"/>
+      <c r="V36" s="72"/>
+      <c r="W36" s="72"/>
+      <c r="X36" s="72"/>
+      <c r="Y36" s="72"/>
+      <c r="Z36" s="72"/>
+      <c r="AA36" s="73"/>
       <c r="AB36" s="16"/>
       <c r="AC36" s="16"/>
       <c r="AD36" s="16"/>
@@ -4680,33 +4707,33 @@
       <c r="AF36" s="16"/>
     </row>
     <row r="37" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="122"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="48"/>
-      <c r="D37" s="48"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="125"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="52"/>
-      <c r="K37" s="52"/>
-      <c r="L37" s="52"/>
-      <c r="M37" s="52"/>
-      <c r="N37" s="53"/>
-      <c r="O37" s="106"/>
-      <c r="P37" s="107"/>
-      <c r="Q37" s="107"/>
-      <c r="R37" s="107"/>
-      <c r="S37" s="107"/>
-      <c r="T37" s="107"/>
-      <c r="U37" s="107"/>
-      <c r="V37" s="107"/>
-      <c r="W37" s="107"/>
-      <c r="X37" s="107"/>
-      <c r="Y37" s="107"/>
-      <c r="Z37" s="107"/>
-      <c r="AA37" s="108"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="53"/>
+      <c r="I37" s="53"/>
+      <c r="J37" s="53"/>
+      <c r="K37" s="53"/>
+      <c r="L37" s="53"/>
+      <c r="M37" s="53"/>
+      <c r="N37" s="54"/>
+      <c r="O37" s="71"/>
+      <c r="P37" s="72"/>
+      <c r="Q37" s="72"/>
+      <c r="R37" s="72"/>
+      <c r="S37" s="72"/>
+      <c r="T37" s="72"/>
+      <c r="U37" s="72"/>
+      <c r="V37" s="72"/>
+      <c r="W37" s="72"/>
+      <c r="X37" s="72"/>
+      <c r="Y37" s="72"/>
+      <c r="Z37" s="72"/>
+      <c r="AA37" s="73"/>
       <c r="AB37" s="16"/>
       <c r="AC37" s="16"/>
       <c r="AD37" s="16"/>
@@ -4714,33 +4741,33 @@
       <c r="AF37" s="16"/>
     </row>
     <row r="38" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="122"/>
-      <c r="B38" s="48"/>
-      <c r="C38" s="48"/>
-      <c r="D38" s="48"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
-      <c r="G38" s="125"/>
-      <c r="H38" s="52"/>
-      <c r="I38" s="52"/>
-      <c r="J38" s="52"/>
-      <c r="K38" s="52"/>
-      <c r="L38" s="52"/>
-      <c r="M38" s="52"/>
-      <c r="N38" s="53"/>
-      <c r="O38" s="106"/>
-      <c r="P38" s="107"/>
-      <c r="Q38" s="107"/>
-      <c r="R38" s="107"/>
-      <c r="S38" s="107"/>
-      <c r="T38" s="107"/>
-      <c r="U38" s="107"/>
-      <c r="V38" s="107"/>
-      <c r="W38" s="107"/>
-      <c r="X38" s="107"/>
-      <c r="Y38" s="107"/>
-      <c r="Z38" s="107"/>
-      <c r="AA38" s="108"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="53"/>
+      <c r="L38" s="53"/>
+      <c r="M38" s="53"/>
+      <c r="N38" s="54"/>
+      <c r="O38" s="71"/>
+      <c r="P38" s="72"/>
+      <c r="Q38" s="72"/>
+      <c r="R38" s="72"/>
+      <c r="S38" s="72"/>
+      <c r="T38" s="72"/>
+      <c r="U38" s="72"/>
+      <c r="V38" s="72"/>
+      <c r="W38" s="72"/>
+      <c r="X38" s="72"/>
+      <c r="Y38" s="72"/>
+      <c r="Z38" s="72"/>
+      <c r="AA38" s="73"/>
       <c r="AB38" s="16"/>
       <c r="AC38" s="16"/>
       <c r="AD38" s="16"/>
@@ -4748,33 +4775,33 @@
       <c r="AF38" s="16"/>
     </row>
     <row r="39" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="122"/>
-      <c r="B39" s="48"/>
-      <c r="C39" s="48"/>
-      <c r="D39" s="48"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
-      <c r="G39" s="125"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="52"/>
-      <c r="L39" s="52"/>
-      <c r="M39" s="52"/>
-      <c r="N39" s="53"/>
-      <c r="O39" s="106"/>
-      <c r="P39" s="107"/>
-      <c r="Q39" s="107"/>
-      <c r="R39" s="107"/>
-      <c r="S39" s="107"/>
-      <c r="T39" s="107"/>
-      <c r="U39" s="107"/>
-      <c r="V39" s="107"/>
-      <c r="W39" s="107"/>
-      <c r="X39" s="107"/>
-      <c r="Y39" s="107"/>
-      <c r="Z39" s="107"/>
-      <c r="AA39" s="108"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="53"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="53"/>
+      <c r="L39" s="53"/>
+      <c r="M39" s="53"/>
+      <c r="N39" s="54"/>
+      <c r="O39" s="71"/>
+      <c r="P39" s="72"/>
+      <c r="Q39" s="72"/>
+      <c r="R39" s="72"/>
+      <c r="S39" s="72"/>
+      <c r="T39" s="72"/>
+      <c r="U39" s="72"/>
+      <c r="V39" s="72"/>
+      <c r="W39" s="72"/>
+      <c r="X39" s="72"/>
+      <c r="Y39" s="72"/>
+      <c r="Z39" s="72"/>
+      <c r="AA39" s="73"/>
       <c r="AB39" s="16"/>
       <c r="AC39" s="16"/>
       <c r="AD39" s="16"/>
@@ -4782,33 +4809,33 @@
       <c r="AF39" s="16"/>
     </row>
     <row r="40" spans="1:32" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="122"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="48"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
-      <c r="G40" s="126"/>
-      <c r="H40" s="120"/>
-      <c r="I40" s="120"/>
-      <c r="J40" s="120"/>
-      <c r="K40" s="120"/>
-      <c r="L40" s="120"/>
-      <c r="M40" s="120"/>
-      <c r="N40" s="121"/>
-      <c r="O40" s="109"/>
-      <c r="P40" s="110"/>
-      <c r="Q40" s="110"/>
-      <c r="R40" s="110"/>
-      <c r="S40" s="110"/>
-      <c r="T40" s="110"/>
-      <c r="U40" s="110"/>
-      <c r="V40" s="110"/>
-      <c r="W40" s="110"/>
-      <c r="X40" s="110"/>
-      <c r="Y40" s="110"/>
-      <c r="Z40" s="110"/>
-      <c r="AA40" s="111"/>
+      <c r="A40" s="41"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="66"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
+      <c r="K40" s="39"/>
+      <c r="L40" s="39"/>
+      <c r="M40" s="39"/>
+      <c r="N40" s="40"/>
+      <c r="O40" s="74"/>
+      <c r="P40" s="75"/>
+      <c r="Q40" s="75"/>
+      <c r="R40" s="75"/>
+      <c r="S40" s="75"/>
+      <c r="T40" s="75"/>
+      <c r="U40" s="75"/>
+      <c r="V40" s="75"/>
+      <c r="W40" s="75"/>
+      <c r="X40" s="75"/>
+      <c r="Y40" s="75"/>
+      <c r="Z40" s="75"/>
+      <c r="AA40" s="76"/>
       <c r="AB40" s="16"/>
       <c r="AC40" s="16"/>
       <c r="AD40" s="16"/>
@@ -4816,35 +4843,35 @@
       <c r="AF40" s="16"/>
     </row>
     <row r="41" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="122"/>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="98" t="s">
+      <c r="A41" s="41"/>
+      <c r="B41" s="66"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="66"/>
+      <c r="G41" s="114" t="s">
         <v>41</v>
       </c>
-      <c r="H41" s="99"/>
-      <c r="I41" s="99"/>
-      <c r="J41" s="99"/>
-      <c r="K41" s="99"/>
-      <c r="L41" s="99"/>
-      <c r="M41" s="99"/>
-      <c r="N41" s="99"/>
-      <c r="O41" s="99"/>
-      <c r="P41" s="99"/>
-      <c r="Q41" s="99"/>
-      <c r="R41" s="99"/>
-      <c r="S41" s="99"/>
-      <c r="T41" s="99"/>
-      <c r="U41" s="99"/>
-      <c r="V41" s="99"/>
-      <c r="W41" s="99"/>
-      <c r="X41" s="99"/>
-      <c r="Y41" s="99"/>
-      <c r="Z41" s="99"/>
-      <c r="AA41" s="100"/>
+      <c r="H41" s="115"/>
+      <c r="I41" s="115"/>
+      <c r="J41" s="115"/>
+      <c r="K41" s="115"/>
+      <c r="L41" s="115"/>
+      <c r="M41" s="115"/>
+      <c r="N41" s="115"/>
+      <c r="O41" s="115"/>
+      <c r="P41" s="115"/>
+      <c r="Q41" s="115"/>
+      <c r="R41" s="115"/>
+      <c r="S41" s="115"/>
+      <c r="T41" s="115"/>
+      <c r="U41" s="115"/>
+      <c r="V41" s="115"/>
+      <c r="W41" s="115"/>
+      <c r="X41" s="115"/>
+      <c r="Y41" s="115"/>
+      <c r="Z41" s="115"/>
+      <c r="AA41" s="116"/>
       <c r="AB41" s="16"/>
       <c r="AC41" s="16"/>
       <c r="AD41" s="16"/>
@@ -4852,35 +4879,35 @@
       <c r="AF41" s="16"/>
     </row>
     <row r="42" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="122"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="101" t="s">
+      <c r="A42" s="41"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="66"/>
+      <c r="G42" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="H42" s="102"/>
-      <c r="I42" s="102"/>
-      <c r="J42" s="102"/>
-      <c r="K42" s="102"/>
-      <c r="L42" s="102"/>
-      <c r="M42" s="102"/>
-      <c r="N42" s="102"/>
-      <c r="O42" s="102"/>
-      <c r="P42" s="102"/>
-      <c r="Q42" s="102"/>
-      <c r="R42" s="102"/>
-      <c r="S42" s="102"/>
-      <c r="T42" s="102"/>
-      <c r="U42" s="102"/>
-      <c r="V42" s="102"/>
-      <c r="W42" s="102"/>
-      <c r="X42" s="102"/>
-      <c r="Y42" s="102"/>
-      <c r="Z42" s="102"/>
-      <c r="AA42" s="67"/>
+      <c r="H42" s="57"/>
+      <c r="I42" s="57"/>
+      <c r="J42" s="57"/>
+      <c r="K42" s="57"/>
+      <c r="L42" s="57"/>
+      <c r="M42" s="57"/>
+      <c r="N42" s="57"/>
+      <c r="O42" s="57"/>
+      <c r="P42" s="57"/>
+      <c r="Q42" s="57"/>
+      <c r="R42" s="57"/>
+      <c r="S42" s="57"/>
+      <c r="T42" s="57"/>
+      <c r="U42" s="57"/>
+      <c r="V42" s="57"/>
+      <c r="W42" s="57"/>
+      <c r="X42" s="57"/>
+      <c r="Y42" s="57"/>
+      <c r="Z42" s="57"/>
+      <c r="AA42" s="58"/>
       <c r="AB42" s="16"/>
       <c r="AC42" s="16"/>
       <c r="AD42" s="16"/>
@@ -4888,33 +4915,33 @@
       <c r="AF42" s="16"/>
     </row>
     <row r="43" spans="1:32" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="122"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="101"/>
-      <c r="H43" s="102"/>
-      <c r="I43" s="102"/>
-      <c r="J43" s="102"/>
-      <c r="K43" s="102"/>
-      <c r="L43" s="102"/>
-      <c r="M43" s="102"/>
-      <c r="N43" s="102"/>
-      <c r="O43" s="102"/>
-      <c r="P43" s="102"/>
-      <c r="Q43" s="102"/>
-      <c r="R43" s="102"/>
-      <c r="S43" s="102"/>
-      <c r="T43" s="102"/>
-      <c r="U43" s="102"/>
-      <c r="V43" s="102"/>
-      <c r="W43" s="102"/>
-      <c r="X43" s="102"/>
-      <c r="Y43" s="102"/>
-      <c r="Z43" s="102"/>
-      <c r="AA43" s="67"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="56"/>
+      <c r="H43" s="57"/>
+      <c r="I43" s="57"/>
+      <c r="J43" s="57"/>
+      <c r="K43" s="57"/>
+      <c r="L43" s="57"/>
+      <c r="M43" s="57"/>
+      <c r="N43" s="57"/>
+      <c r="O43" s="57"/>
+      <c r="P43" s="57"/>
+      <c r="Q43" s="57"/>
+      <c r="R43" s="57"/>
+      <c r="S43" s="57"/>
+      <c r="T43" s="57"/>
+      <c r="U43" s="57"/>
+      <c r="V43" s="57"/>
+      <c r="W43" s="57"/>
+      <c r="X43" s="57"/>
+      <c r="Y43" s="57"/>
+      <c r="Z43" s="57"/>
+      <c r="AA43" s="58"/>
       <c r="AB43" s="16"/>
       <c r="AC43" s="16"/>
       <c r="AD43" s="16"/>
@@ -4922,33 +4949,33 @@
       <c r="AF43" s="16"/>
     </row>
     <row r="44" spans="1:32" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="122"/>
-      <c r="B44" s="49"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="103"/>
-      <c r="H44" s="104"/>
-      <c r="I44" s="104"/>
-      <c r="J44" s="104"/>
-      <c r="K44" s="104"/>
-      <c r="L44" s="104"/>
-      <c r="M44" s="104"/>
-      <c r="N44" s="104"/>
-      <c r="O44" s="104"/>
-      <c r="P44" s="104"/>
-      <c r="Q44" s="104"/>
-      <c r="R44" s="104"/>
-      <c r="S44" s="104"/>
-      <c r="T44" s="104"/>
-      <c r="U44" s="104"/>
-      <c r="V44" s="104"/>
-      <c r="W44" s="104"/>
-      <c r="X44" s="104"/>
-      <c r="Y44" s="104"/>
-      <c r="Z44" s="104"/>
-      <c r="AA44" s="105"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="67"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="60"/>
+      <c r="I44" s="60"/>
+      <c r="J44" s="60"/>
+      <c r="K44" s="60"/>
+      <c r="L44" s="60"/>
+      <c r="M44" s="60"/>
+      <c r="N44" s="60"/>
+      <c r="O44" s="60"/>
+      <c r="P44" s="60"/>
+      <c r="Q44" s="60"/>
+      <c r="R44" s="60"/>
+      <c r="S44" s="60"/>
+      <c r="T44" s="60"/>
+      <c r="U44" s="60"/>
+      <c r="V44" s="60"/>
+      <c r="W44" s="60"/>
+      <c r="X44" s="60"/>
+      <c r="Y44" s="60"/>
+      <c r="Z44" s="60"/>
+      <c r="AA44" s="61"/>
       <c r="AB44" s="16"/>
       <c r="AC44" s="16"/>
       <c r="AD44" s="16"/>
@@ -4956,789 +4983,849 @@
       <c r="AF44" s="16"/>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A45" s="122"/>
-      <c r="B45" s="118"/>
-      <c r="C45" s="118"/>
-      <c r="D45" s="118"/>
-      <c r="E45" s="118"/>
-      <c r="F45" s="118"/>
-      <c r="G45" s="118"/>
-      <c r="H45" s="118"/>
-      <c r="I45" s="118"/>
-      <c r="J45" s="118"/>
-      <c r="K45" s="118"/>
-      <c r="L45" s="118"/>
-      <c r="M45" s="118"/>
-      <c r="N45" s="118"/>
-      <c r="O45" s="118"/>
-      <c r="P45" s="118"/>
-      <c r="Q45" s="118"/>
-      <c r="R45" s="118"/>
-      <c r="S45" s="118"/>
-      <c r="T45" s="118"/>
-      <c r="U45" s="118"/>
-      <c r="V45" s="118"/>
-      <c r="W45" s="118"/>
-      <c r="X45" s="118"/>
-      <c r="Y45" s="118"/>
-      <c r="Z45" s="118"/>
-      <c r="AA45" s="118"/>
-      <c r="AB45" s="118"/>
-      <c r="AC45" s="118"/>
-      <c r="AD45" s="118"/>
-      <c r="AE45" s="118"/>
-      <c r="AF45" s="118"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="37"/>
+      <c r="D45" s="37"/>
+      <c r="E45" s="37"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
+      <c r="J45" s="37"/>
+      <c r="K45" s="37"/>
+      <c r="L45" s="37"/>
+      <c r="M45" s="37"/>
+      <c r="N45" s="37"/>
+      <c r="O45" s="37"/>
+      <c r="P45" s="37"/>
+      <c r="Q45" s="37"/>
+      <c r="R45" s="37"/>
+      <c r="S45" s="37"/>
+      <c r="T45" s="37"/>
+      <c r="U45" s="37"/>
+      <c r="V45" s="37"/>
+      <c r="W45" s="37"/>
+      <c r="X45" s="37"/>
+      <c r="Y45" s="37"/>
+      <c r="Z45" s="37"/>
+      <c r="AA45" s="37"/>
+      <c r="AB45" s="37"/>
+      <c r="AC45" s="37"/>
+      <c r="AD45" s="37"/>
+      <c r="AE45" s="37"/>
+      <c r="AF45" s="37"/>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A46" s="118"/>
-      <c r="B46" s="118"/>
-      <c r="C46" s="118"/>
-      <c r="D46" s="118"/>
-      <c r="E46" s="118"/>
-      <c r="F46" s="118"/>
-      <c r="G46" s="118"/>
-      <c r="H46" s="118"/>
-      <c r="I46" s="118"/>
-      <c r="J46" s="118"/>
-      <c r="K46" s="118"/>
-      <c r="L46" s="118"/>
-      <c r="M46" s="118"/>
-      <c r="N46" s="118"/>
-      <c r="O46" s="118"/>
-      <c r="P46" s="118"/>
-      <c r="Q46" s="118"/>
-      <c r="R46" s="118"/>
-      <c r="S46" s="118"/>
-      <c r="T46" s="118"/>
-      <c r="U46" s="118"/>
-      <c r="V46" s="118"/>
-      <c r="W46" s="118"/>
-      <c r="X46" s="118"/>
-      <c r="Y46" s="118"/>
-      <c r="Z46" s="118"/>
-      <c r="AA46" s="118"/>
-      <c r="AB46" s="118"/>
-      <c r="AC46" s="118"/>
-      <c r="AD46" s="118"/>
-      <c r="AE46" s="118"/>
-      <c r="AF46" s="118"/>
+      <c r="A46" s="37"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
+      <c r="K46" s="37"/>
+      <c r="L46" s="37"/>
+      <c r="M46" s="37"/>
+      <c r="N46" s="37"/>
+      <c r="O46" s="37"/>
+      <c r="P46" s="37"/>
+      <c r="Q46" s="37"/>
+      <c r="R46" s="37"/>
+      <c r="S46" s="37"/>
+      <c r="T46" s="37"/>
+      <c r="U46" s="37"/>
+      <c r="V46" s="37"/>
+      <c r="W46" s="37"/>
+      <c r="X46" s="37"/>
+      <c r="Y46" s="37"/>
+      <c r="Z46" s="37"/>
+      <c r="AA46" s="37"/>
+      <c r="AB46" s="37"/>
+      <c r="AC46" s="37"/>
+      <c r="AD46" s="37"/>
+      <c r="AE46" s="37"/>
+      <c r="AF46" s="37"/>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A47" s="118"/>
-      <c r="B47" s="118"/>
-      <c r="C47" s="118"/>
-      <c r="D47" s="118"/>
-      <c r="E47" s="118"/>
-      <c r="F47" s="118"/>
-      <c r="G47" s="118"/>
-      <c r="H47" s="118"/>
-      <c r="I47" s="118"/>
-      <c r="J47" s="118"/>
-      <c r="K47" s="118"/>
-      <c r="L47" s="118"/>
-      <c r="M47" s="118"/>
-      <c r="N47" s="118"/>
-      <c r="O47" s="118"/>
-      <c r="P47" s="118"/>
-      <c r="Q47" s="118"/>
-      <c r="R47" s="118"/>
-      <c r="S47" s="118"/>
-      <c r="T47" s="118"/>
-      <c r="U47" s="118"/>
-      <c r="V47" s="118"/>
-      <c r="W47" s="118"/>
-      <c r="X47" s="118"/>
-      <c r="Y47" s="118"/>
-      <c r="Z47" s="118"/>
-      <c r="AA47" s="118"/>
-      <c r="AB47" s="118"/>
-      <c r="AC47" s="118"/>
-      <c r="AD47" s="118"/>
-      <c r="AE47" s="118"/>
-      <c r="AF47" s="118"/>
+      <c r="A47" s="37"/>
+      <c r="B47" s="37"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="37"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="37"/>
+      <c r="K47" s="37"/>
+      <c r="L47" s="37"/>
+      <c r="M47" s="37"/>
+      <c r="N47" s="37"/>
+      <c r="O47" s="37"/>
+      <c r="P47" s="37"/>
+      <c r="Q47" s="37"/>
+      <c r="R47" s="37"/>
+      <c r="S47" s="37"/>
+      <c r="T47" s="37"/>
+      <c r="U47" s="37"/>
+      <c r="V47" s="37"/>
+      <c r="W47" s="37"/>
+      <c r="X47" s="37"/>
+      <c r="Y47" s="37"/>
+      <c r="Z47" s="37"/>
+      <c r="AA47" s="37"/>
+      <c r="AB47" s="37"/>
+      <c r="AC47" s="37"/>
+      <c r="AD47" s="37"/>
+      <c r="AE47" s="37"/>
+      <c r="AF47" s="37"/>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A48" s="118"/>
-      <c r="B48" s="118"/>
-      <c r="C48" s="118"/>
-      <c r="D48" s="118"/>
-      <c r="E48" s="118"/>
-      <c r="F48" s="118"/>
-      <c r="G48" s="118"/>
-      <c r="H48" s="118"/>
-      <c r="I48" s="118"/>
-      <c r="J48" s="118"/>
-      <c r="K48" s="118"/>
-      <c r="L48" s="118"/>
-      <c r="M48" s="118"/>
-      <c r="N48" s="118"/>
-      <c r="O48" s="118"/>
-      <c r="P48" s="118"/>
-      <c r="Q48" s="118"/>
-      <c r="R48" s="118"/>
-      <c r="S48" s="118"/>
-      <c r="T48" s="118"/>
-      <c r="U48" s="118"/>
-      <c r="V48" s="118"/>
-      <c r="W48" s="118"/>
-      <c r="X48" s="118"/>
-      <c r="Y48" s="118"/>
-      <c r="Z48" s="118"/>
-      <c r="AA48" s="118"/>
-      <c r="AB48" s="118"/>
-      <c r="AC48" s="118"/>
-      <c r="AD48" s="118"/>
-      <c r="AE48" s="118"/>
-      <c r="AF48" s="118"/>
+      <c r="A48" s="37"/>
+      <c r="B48" s="37"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="37"/>
+      <c r="J48" s="37"/>
+      <c r="K48" s="37"/>
+      <c r="L48" s="37"/>
+      <c r="M48" s="37"/>
+      <c r="N48" s="37"/>
+      <c r="O48" s="37"/>
+      <c r="P48" s="37"/>
+      <c r="Q48" s="37"/>
+      <c r="R48" s="37"/>
+      <c r="S48" s="37"/>
+      <c r="T48" s="37"/>
+      <c r="U48" s="37"/>
+      <c r="V48" s="37"/>
+      <c r="W48" s="37"/>
+      <c r="X48" s="37"/>
+      <c r="Y48" s="37"/>
+      <c r="Z48" s="37"/>
+      <c r="AA48" s="37"/>
+      <c r="AB48" s="37"/>
+      <c r="AC48" s="37"/>
+      <c r="AD48" s="37"/>
+      <c r="AE48" s="37"/>
+      <c r="AF48" s="37"/>
     </row>
     <row r="49" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A49" s="118"/>
-      <c r="B49" s="118"/>
-      <c r="C49" s="118"/>
-      <c r="D49" s="118"/>
-      <c r="E49" s="118"/>
-      <c r="F49" s="118"/>
-      <c r="G49" s="118"/>
-      <c r="H49" s="118"/>
-      <c r="I49" s="118"/>
-      <c r="J49" s="118"/>
-      <c r="K49" s="118"/>
-      <c r="L49" s="118"/>
-      <c r="M49" s="118"/>
-      <c r="N49" s="118"/>
-      <c r="O49" s="118"/>
-      <c r="P49" s="118"/>
-      <c r="Q49" s="118"/>
-      <c r="R49" s="118"/>
-      <c r="S49" s="118"/>
-      <c r="T49" s="118"/>
-      <c r="U49" s="118"/>
-      <c r="V49" s="118"/>
-      <c r="W49" s="118"/>
-      <c r="X49" s="118"/>
-      <c r="Y49" s="118"/>
-      <c r="Z49" s="118"/>
-      <c r="AA49" s="118"/>
-      <c r="AB49" s="118"/>
-      <c r="AC49" s="118"/>
-      <c r="AD49" s="118"/>
-      <c r="AE49" s="118"/>
-      <c r="AF49" s="118"/>
+      <c r="A49" s="37"/>
+      <c r="B49" s="37"/>
+      <c r="C49" s="37"/>
+      <c r="D49" s="37"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="37"/>
+      <c r="J49" s="37"/>
+      <c r="K49" s="37"/>
+      <c r="L49" s="37"/>
+      <c r="M49" s="37"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="37"/>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
+      <c r="S49" s="37"/>
+      <c r="T49" s="37"/>
+      <c r="U49" s="37"/>
+      <c r="V49" s="37"/>
+      <c r="W49" s="37"/>
+      <c r="X49" s="37"/>
+      <c r="Y49" s="37"/>
+      <c r="Z49" s="37"/>
+      <c r="AA49" s="37"/>
+      <c r="AB49" s="37"/>
+      <c r="AC49" s="37"/>
+      <c r="AD49" s="37"/>
+      <c r="AE49" s="37"/>
+      <c r="AF49" s="37"/>
     </row>
     <row r="50" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A50" s="118"/>
-      <c r="B50" s="118"/>
-      <c r="C50" s="118"/>
-      <c r="D50" s="118"/>
-      <c r="E50" s="118"/>
-      <c r="F50" s="118"/>
-      <c r="G50" s="118"/>
-      <c r="H50" s="118"/>
-      <c r="I50" s="118"/>
-      <c r="J50" s="118"/>
-      <c r="K50" s="118"/>
-      <c r="L50" s="118"/>
-      <c r="M50" s="118"/>
-      <c r="N50" s="118"/>
-      <c r="O50" s="118"/>
-      <c r="P50" s="118"/>
-      <c r="Q50" s="118"/>
-      <c r="R50" s="118"/>
-      <c r="S50" s="118"/>
-      <c r="T50" s="118"/>
-      <c r="U50" s="118"/>
-      <c r="V50" s="118"/>
-      <c r="W50" s="118"/>
-      <c r="X50" s="118"/>
-      <c r="Y50" s="118"/>
-      <c r="Z50" s="118"/>
-      <c r="AA50" s="118"/>
-      <c r="AB50" s="118"/>
-      <c r="AC50" s="118"/>
-      <c r="AD50" s="118"/>
-      <c r="AE50" s="118"/>
-      <c r="AF50" s="118"/>
+      <c r="A50" s="37"/>
+      <c r="B50" s="37"/>
+      <c r="C50" s="37"/>
+      <c r="D50" s="37"/>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="37"/>
+      <c r="J50" s="37"/>
+      <c r="K50" s="37"/>
+      <c r="L50" s="37"/>
+      <c r="M50" s="37"/>
+      <c r="N50" s="37"/>
+      <c r="O50" s="37"/>
+      <c r="P50" s="37"/>
+      <c r="Q50" s="37"/>
+      <c r="R50" s="37"/>
+      <c r="S50" s="37"/>
+      <c r="T50" s="37"/>
+      <c r="U50" s="37"/>
+      <c r="V50" s="37"/>
+      <c r="W50" s="37"/>
+      <c r="X50" s="37"/>
+      <c r="Y50" s="37"/>
+      <c r="Z50" s="37"/>
+      <c r="AA50" s="37"/>
+      <c r="AB50" s="37"/>
+      <c r="AC50" s="37"/>
+      <c r="AD50" s="37"/>
+      <c r="AE50" s="37"/>
+      <c r="AF50" s="37"/>
     </row>
     <row r="51" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A51" s="118"/>
-      <c r="B51" s="118"/>
-      <c r="C51" s="118"/>
-      <c r="D51" s="118"/>
-      <c r="E51" s="118"/>
-      <c r="F51" s="118"/>
-      <c r="G51" s="118"/>
-      <c r="H51" s="118"/>
-      <c r="I51" s="118"/>
-      <c r="J51" s="118"/>
-      <c r="K51" s="118"/>
-      <c r="L51" s="118"/>
-      <c r="M51" s="118"/>
-      <c r="N51" s="118"/>
-      <c r="O51" s="118"/>
-      <c r="P51" s="118"/>
-      <c r="Q51" s="118"/>
-      <c r="R51" s="118"/>
-      <c r="S51" s="118"/>
-      <c r="T51" s="118"/>
-      <c r="U51" s="118"/>
-      <c r="V51" s="118"/>
-      <c r="W51" s="118"/>
-      <c r="X51" s="118"/>
-      <c r="Y51" s="118"/>
-      <c r="Z51" s="118"/>
-      <c r="AA51" s="118"/>
-      <c r="AB51" s="118"/>
-      <c r="AC51" s="118"/>
-      <c r="AD51" s="118"/>
-      <c r="AE51" s="118"/>
-      <c r="AF51" s="118"/>
+      <c r="A51" s="37"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="37"/>
+      <c r="J51" s="37"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
+      <c r="N51" s="37"/>
+      <c r="O51" s="37"/>
+      <c r="P51" s="37"/>
+      <c r="Q51" s="37"/>
+      <c r="R51" s="37"/>
+      <c r="S51" s="37"/>
+      <c r="T51" s="37"/>
+      <c r="U51" s="37"/>
+      <c r="V51" s="37"/>
+      <c r="W51" s="37"/>
+      <c r="X51" s="37"/>
+      <c r="Y51" s="37"/>
+      <c r="Z51" s="37"/>
+      <c r="AA51" s="37"/>
+      <c r="AB51" s="37"/>
+      <c r="AC51" s="37"/>
+      <c r="AD51" s="37"/>
+      <c r="AE51" s="37"/>
+      <c r="AF51" s="37"/>
     </row>
     <row r="52" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A52" s="118"/>
-      <c r="B52" s="118"/>
-      <c r="C52" s="118"/>
-      <c r="D52" s="118"/>
-      <c r="E52" s="118"/>
-      <c r="F52" s="118"/>
-      <c r="G52" s="118"/>
-      <c r="H52" s="118"/>
-      <c r="I52" s="118"/>
-      <c r="J52" s="118"/>
-      <c r="K52" s="118"/>
-      <c r="L52" s="118"/>
-      <c r="M52" s="118"/>
-      <c r="N52" s="118"/>
-      <c r="O52" s="118"/>
-      <c r="P52" s="118"/>
-      <c r="Q52" s="118"/>
-      <c r="R52" s="118"/>
-      <c r="S52" s="118"/>
-      <c r="T52" s="118"/>
-      <c r="U52" s="118"/>
-      <c r="V52" s="118"/>
-      <c r="W52" s="118"/>
-      <c r="X52" s="118"/>
-      <c r="Y52" s="118"/>
-      <c r="Z52" s="118"/>
-      <c r="AA52" s="118"/>
-      <c r="AB52" s="118"/>
-      <c r="AC52" s="118"/>
-      <c r="AD52" s="118"/>
-      <c r="AE52" s="118"/>
-      <c r="AF52" s="118"/>
+      <c r="A52" s="37"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="37"/>
+      <c r="J52" s="37"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="37"/>
+      <c r="M52" s="37"/>
+      <c r="N52" s="37"/>
+      <c r="O52" s="37"/>
+      <c r="P52" s="37"/>
+      <c r="Q52" s="37"/>
+      <c r="R52" s="37"/>
+      <c r="S52" s="37"/>
+      <c r="T52" s="37"/>
+      <c r="U52" s="37"/>
+      <c r="V52" s="37"/>
+      <c r="W52" s="37"/>
+      <c r="X52" s="37"/>
+      <c r="Y52" s="37"/>
+      <c r="Z52" s="37"/>
+      <c r="AA52" s="37"/>
+      <c r="AB52" s="37"/>
+      <c r="AC52" s="37"/>
+      <c r="AD52" s="37"/>
+      <c r="AE52" s="37"/>
+      <c r="AF52" s="37"/>
     </row>
     <row r="53" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A53" s="118"/>
-      <c r="B53" s="118"/>
-      <c r="C53" s="118"/>
-      <c r="D53" s="118"/>
-      <c r="E53" s="118"/>
-      <c r="F53" s="118"/>
-      <c r="G53" s="118"/>
-      <c r="H53" s="118"/>
-      <c r="I53" s="118"/>
-      <c r="J53" s="118"/>
-      <c r="K53" s="118"/>
-      <c r="L53" s="118"/>
-      <c r="M53" s="118"/>
-      <c r="N53" s="118"/>
-      <c r="O53" s="118"/>
-      <c r="P53" s="118"/>
-      <c r="Q53" s="118"/>
-      <c r="R53" s="118"/>
-      <c r="S53" s="118"/>
-      <c r="T53" s="118"/>
-      <c r="U53" s="118"/>
-      <c r="V53" s="118"/>
-      <c r="W53" s="118"/>
-      <c r="X53" s="118"/>
-      <c r="Y53" s="118"/>
-      <c r="Z53" s="118"/>
-      <c r="AA53" s="118"/>
-      <c r="AB53" s="118"/>
-      <c r="AC53" s="118"/>
-      <c r="AD53" s="118"/>
-      <c r="AE53" s="118"/>
-      <c r="AF53" s="118"/>
+      <c r="A53" s="37"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="37"/>
+      <c r="M53" s="37"/>
+      <c r="N53" s="37"/>
+      <c r="O53" s="37"/>
+      <c r="P53" s="37"/>
+      <c r="Q53" s="37"/>
+      <c r="R53" s="37"/>
+      <c r="S53" s="37"/>
+      <c r="T53" s="37"/>
+      <c r="U53" s="37"/>
+      <c r="V53" s="37"/>
+      <c r="W53" s="37"/>
+      <c r="X53" s="37"/>
+      <c r="Y53" s="37"/>
+      <c r="Z53" s="37"/>
+      <c r="AA53" s="37"/>
+      <c r="AB53" s="37"/>
+      <c r="AC53" s="37"/>
+      <c r="AD53" s="37"/>
+      <c r="AE53" s="37"/>
+      <c r="AF53" s="37"/>
     </row>
     <row r="54" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A54" s="118"/>
-      <c r="B54" s="118"/>
-      <c r="C54" s="118"/>
-      <c r="D54" s="118"/>
-      <c r="E54" s="118"/>
-      <c r="F54" s="118"/>
-      <c r="G54" s="118"/>
-      <c r="H54" s="118"/>
-      <c r="I54" s="118"/>
-      <c r="J54" s="118"/>
-      <c r="K54" s="118"/>
-      <c r="L54" s="118"/>
-      <c r="M54" s="118"/>
-      <c r="N54" s="118"/>
-      <c r="O54" s="118"/>
-      <c r="P54" s="118"/>
-      <c r="Q54" s="118"/>
-      <c r="R54" s="118"/>
-      <c r="S54" s="118"/>
-      <c r="T54" s="118"/>
-      <c r="U54" s="118"/>
-      <c r="V54" s="118"/>
-      <c r="W54" s="118"/>
-      <c r="X54" s="118"/>
-      <c r="Y54" s="118"/>
-      <c r="Z54" s="118"/>
-      <c r="AA54" s="118"/>
-      <c r="AB54" s="118"/>
-      <c r="AC54" s="118"/>
-      <c r="AD54" s="118"/>
-      <c r="AE54" s="118"/>
-      <c r="AF54" s="118"/>
+      <c r="A54" s="37"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="37"/>
+      <c r="L54" s="37"/>
+      <c r="M54" s="37"/>
+      <c r="N54" s="37"/>
+      <c r="O54" s="37"/>
+      <c r="P54" s="37"/>
+      <c r="Q54" s="37"/>
+      <c r="R54" s="37"/>
+      <c r="S54" s="37"/>
+      <c r="T54" s="37"/>
+      <c r="U54" s="37"/>
+      <c r="V54" s="37"/>
+      <c r="W54" s="37"/>
+      <c r="X54" s="37"/>
+      <c r="Y54" s="37"/>
+      <c r="Z54" s="37"/>
+      <c r="AA54" s="37"/>
+      <c r="AB54" s="37"/>
+      <c r="AC54" s="37"/>
+      <c r="AD54" s="37"/>
+      <c r="AE54" s="37"/>
+      <c r="AF54" s="37"/>
     </row>
     <row r="55" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A55" s="118"/>
-      <c r="B55" s="118"/>
-      <c r="C55" s="118"/>
-      <c r="D55" s="118"/>
-      <c r="E55" s="118"/>
-      <c r="F55" s="118"/>
-      <c r="G55" s="118"/>
-      <c r="H55" s="118"/>
-      <c r="I55" s="118"/>
-      <c r="J55" s="118"/>
-      <c r="K55" s="118"/>
-      <c r="L55" s="118"/>
-      <c r="M55" s="118"/>
-      <c r="N55" s="118"/>
-      <c r="O55" s="118"/>
-      <c r="P55" s="118"/>
-      <c r="Q55" s="118"/>
-      <c r="R55" s="118"/>
-      <c r="S55" s="118"/>
-      <c r="T55" s="118"/>
-      <c r="U55" s="118"/>
-      <c r="V55" s="118"/>
-      <c r="W55" s="118"/>
-      <c r="X55" s="118"/>
-      <c r="Y55" s="118"/>
-      <c r="Z55" s="118"/>
-      <c r="AA55" s="118"/>
-      <c r="AB55" s="118"/>
-      <c r="AC55" s="118"/>
-      <c r="AD55" s="118"/>
-      <c r="AE55" s="118"/>
-      <c r="AF55" s="118"/>
+      <c r="A55" s="37"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="37"/>
+      <c r="M55" s="37"/>
+      <c r="N55" s="37"/>
+      <c r="O55" s="37"/>
+      <c r="P55" s="37"/>
+      <c r="Q55" s="37"/>
+      <c r="R55" s="37"/>
+      <c r="S55" s="37"/>
+      <c r="T55" s="37"/>
+      <c r="U55" s="37"/>
+      <c r="V55" s="37"/>
+      <c r="W55" s="37"/>
+      <c r="X55" s="37"/>
+      <c r="Y55" s="37"/>
+      <c r="Z55" s="37"/>
+      <c r="AA55" s="37"/>
+      <c r="AB55" s="37"/>
+      <c r="AC55" s="37"/>
+      <c r="AD55" s="37"/>
+      <c r="AE55" s="37"/>
+      <c r="AF55" s="37"/>
     </row>
     <row r="56" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A56" s="118"/>
-      <c r="B56" s="118"/>
-      <c r="C56" s="118"/>
-      <c r="D56" s="118"/>
-      <c r="E56" s="118"/>
-      <c r="F56" s="118"/>
-      <c r="G56" s="118"/>
-      <c r="H56" s="118"/>
-      <c r="I56" s="118"/>
-      <c r="J56" s="118"/>
-      <c r="K56" s="118"/>
-      <c r="L56" s="118"/>
-      <c r="M56" s="118"/>
-      <c r="N56" s="118"/>
-      <c r="O56" s="118"/>
-      <c r="P56" s="118"/>
-      <c r="Q56" s="118"/>
-      <c r="R56" s="118"/>
-      <c r="S56" s="118"/>
-      <c r="T56" s="118"/>
-      <c r="U56" s="118"/>
-      <c r="V56" s="118"/>
-      <c r="W56" s="118"/>
-      <c r="X56" s="118"/>
-      <c r="Y56" s="118"/>
-      <c r="Z56" s="118"/>
-      <c r="AA56" s="118"/>
-      <c r="AB56" s="118"/>
-      <c r="AC56" s="118"/>
-      <c r="AD56" s="118"/>
-      <c r="AE56" s="118"/>
-      <c r="AF56" s="118"/>
+      <c r="A56" s="37"/>
+      <c r="B56" s="37"/>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="37"/>
+      <c r="H56" s="37"/>
+      <c r="I56" s="37"/>
+      <c r="J56" s="37"/>
+      <c r="K56" s="37"/>
+      <c r="L56" s="37"/>
+      <c r="M56" s="37"/>
+      <c r="N56" s="37"/>
+      <c r="O56" s="37"/>
+      <c r="P56" s="37"/>
+      <c r="Q56" s="37"/>
+      <c r="R56" s="37"/>
+      <c r="S56" s="37"/>
+      <c r="T56" s="37"/>
+      <c r="U56" s="37"/>
+      <c r="V56" s="37"/>
+      <c r="W56" s="37"/>
+      <c r="X56" s="37"/>
+      <c r="Y56" s="37"/>
+      <c r="Z56" s="37"/>
+      <c r="AA56" s="37"/>
+      <c r="AB56" s="37"/>
+      <c r="AC56" s="37"/>
+      <c r="AD56" s="37"/>
+      <c r="AE56" s="37"/>
+      <c r="AF56" s="37"/>
     </row>
     <row r="57" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A57" s="118"/>
-      <c r="B57" s="118"/>
-      <c r="C57" s="118"/>
-      <c r="D57" s="118"/>
-      <c r="E57" s="118"/>
-      <c r="F57" s="118"/>
-      <c r="G57" s="118"/>
-      <c r="H57" s="118"/>
-      <c r="I57" s="118"/>
-      <c r="J57" s="118"/>
-      <c r="K57" s="118"/>
-      <c r="L57" s="118"/>
-      <c r="M57" s="118"/>
-      <c r="N57" s="118"/>
-      <c r="O57" s="118"/>
-      <c r="P57" s="118"/>
-      <c r="Q57" s="118"/>
-      <c r="R57" s="118"/>
-      <c r="S57" s="118"/>
-      <c r="T57" s="118"/>
-      <c r="U57" s="118"/>
-      <c r="V57" s="118"/>
-      <c r="W57" s="118"/>
-      <c r="X57" s="118"/>
-      <c r="Y57" s="118"/>
-      <c r="Z57" s="118"/>
-      <c r="AA57" s="118"/>
-      <c r="AB57" s="118"/>
-      <c r="AC57" s="118"/>
-      <c r="AD57" s="118"/>
-      <c r="AE57" s="118"/>
-      <c r="AF57" s="118"/>
+      <c r="A57" s="37"/>
+      <c r="B57" s="37"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="37"/>
+      <c r="J57" s="37"/>
+      <c r="K57" s="37"/>
+      <c r="L57" s="37"/>
+      <c r="M57" s="37"/>
+      <c r="N57" s="37"/>
+      <c r="O57" s="37"/>
+      <c r="P57" s="37"/>
+      <c r="Q57" s="37"/>
+      <c r="R57" s="37"/>
+      <c r="S57" s="37"/>
+      <c r="T57" s="37"/>
+      <c r="U57" s="37"/>
+      <c r="V57" s="37"/>
+      <c r="W57" s="37"/>
+      <c r="X57" s="37"/>
+      <c r="Y57" s="37"/>
+      <c r="Z57" s="37"/>
+      <c r="AA57" s="37"/>
+      <c r="AB57" s="37"/>
+      <c r="AC57" s="37"/>
+      <c r="AD57" s="37"/>
+      <c r="AE57" s="37"/>
+      <c r="AF57" s="37"/>
     </row>
     <row r="58" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A58" s="118"/>
-      <c r="B58" s="118"/>
-      <c r="C58" s="118"/>
-      <c r="D58" s="118"/>
-      <c r="E58" s="118"/>
-      <c r="F58" s="118"/>
-      <c r="G58" s="118"/>
-      <c r="H58" s="118"/>
-      <c r="I58" s="118"/>
-      <c r="J58" s="118"/>
-      <c r="K58" s="118"/>
-      <c r="L58" s="118"/>
-      <c r="M58" s="118"/>
-      <c r="N58" s="118"/>
-      <c r="O58" s="118"/>
-      <c r="P58" s="118"/>
-      <c r="Q58" s="118"/>
-      <c r="R58" s="118"/>
-      <c r="S58" s="118"/>
-      <c r="T58" s="118"/>
-      <c r="U58" s="118"/>
-      <c r="V58" s="118"/>
-      <c r="W58" s="118"/>
-      <c r="X58" s="118"/>
-      <c r="Y58" s="118"/>
-      <c r="Z58" s="118"/>
-      <c r="AA58" s="118"/>
-      <c r="AB58" s="118"/>
-      <c r="AC58" s="118"/>
-      <c r="AD58" s="118"/>
-      <c r="AE58" s="118"/>
-      <c r="AF58" s="118"/>
+      <c r="A58" s="37"/>
+      <c r="B58" s="37"/>
+      <c r="C58" s="37"/>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="37"/>
+      <c r="H58" s="37"/>
+      <c r="I58" s="37"/>
+      <c r="J58" s="37"/>
+      <c r="K58" s="37"/>
+      <c r="L58" s="37"/>
+      <c r="M58" s="37"/>
+      <c r="N58" s="37"/>
+      <c r="O58" s="37"/>
+      <c r="P58" s="37"/>
+      <c r="Q58" s="37"/>
+      <c r="R58" s="37"/>
+      <c r="S58" s="37"/>
+      <c r="T58" s="37"/>
+      <c r="U58" s="37"/>
+      <c r="V58" s="37"/>
+      <c r="W58" s="37"/>
+      <c r="X58" s="37"/>
+      <c r="Y58" s="37"/>
+      <c r="Z58" s="37"/>
+      <c r="AA58" s="37"/>
+      <c r="AB58" s="37"/>
+      <c r="AC58" s="37"/>
+      <c r="AD58" s="37"/>
+      <c r="AE58" s="37"/>
+      <c r="AF58" s="37"/>
     </row>
     <row r="59" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A59" s="118"/>
-      <c r="B59" s="118"/>
-      <c r="C59" s="118"/>
-      <c r="D59" s="118"/>
-      <c r="E59" s="118"/>
-      <c r="F59" s="118"/>
-      <c r="G59" s="118"/>
-      <c r="H59" s="118"/>
-      <c r="I59" s="118"/>
-      <c r="J59" s="118"/>
-      <c r="K59" s="118"/>
-      <c r="L59" s="118"/>
-      <c r="M59" s="118"/>
-      <c r="N59" s="118"/>
-      <c r="O59" s="118"/>
-      <c r="P59" s="118"/>
-      <c r="Q59" s="118"/>
-      <c r="R59" s="118"/>
-      <c r="S59" s="118"/>
-      <c r="T59" s="118"/>
-      <c r="U59" s="118"/>
-      <c r="V59" s="118"/>
-      <c r="W59" s="118"/>
-      <c r="X59" s="118"/>
-      <c r="Y59" s="118"/>
-      <c r="Z59" s="118"/>
-      <c r="AA59" s="118"/>
-      <c r="AB59" s="118"/>
-      <c r="AC59" s="118"/>
-      <c r="AD59" s="118"/>
-      <c r="AE59" s="118"/>
-      <c r="AF59" s="118"/>
+      <c r="A59" s="37"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="37"/>
+      <c r="J59" s="37"/>
+      <c r="K59" s="37"/>
+      <c r="L59" s="37"/>
+      <c r="M59" s="37"/>
+      <c r="N59" s="37"/>
+      <c r="O59" s="37"/>
+      <c r="P59" s="37"/>
+      <c r="Q59" s="37"/>
+      <c r="R59" s="37"/>
+      <c r="S59" s="37"/>
+      <c r="T59" s="37"/>
+      <c r="U59" s="37"/>
+      <c r="V59" s="37"/>
+      <c r="W59" s="37"/>
+      <c r="X59" s="37"/>
+      <c r="Y59" s="37"/>
+      <c r="Z59" s="37"/>
+      <c r="AA59" s="37"/>
+      <c r="AB59" s="37"/>
+      <c r="AC59" s="37"/>
+      <c r="AD59" s="37"/>
+      <c r="AE59" s="37"/>
+      <c r="AF59" s="37"/>
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A60" s="118"/>
-      <c r="B60" s="118"/>
-      <c r="C60" s="118"/>
-      <c r="D60" s="118"/>
-      <c r="E60" s="118"/>
-      <c r="F60" s="118"/>
-      <c r="G60" s="118"/>
-      <c r="H60" s="118"/>
-      <c r="I60" s="118"/>
-      <c r="J60" s="118"/>
-      <c r="K60" s="118"/>
-      <c r="L60" s="118"/>
-      <c r="M60" s="118"/>
-      <c r="N60" s="118"/>
-      <c r="O60" s="118"/>
-      <c r="P60" s="118"/>
-      <c r="Q60" s="118"/>
-      <c r="R60" s="118"/>
-      <c r="S60" s="118"/>
-      <c r="T60" s="118"/>
-      <c r="U60" s="118"/>
-      <c r="V60" s="118"/>
-      <c r="W60" s="118"/>
-      <c r="X60" s="118"/>
-      <c r="Y60" s="118"/>
-      <c r="Z60" s="118"/>
-      <c r="AA60" s="118"/>
-      <c r="AB60" s="118"/>
-      <c r="AC60" s="118"/>
-      <c r="AD60" s="118"/>
-      <c r="AE60" s="118"/>
-      <c r="AF60" s="118"/>
+      <c r="A60" s="37"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="37"/>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="37"/>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
+      <c r="K60" s="37"/>
+      <c r="L60" s="37"/>
+      <c r="M60" s="37"/>
+      <c r="N60" s="37"/>
+      <c r="O60" s="37"/>
+      <c r="P60" s="37"/>
+      <c r="Q60" s="37"/>
+      <c r="R60" s="37"/>
+      <c r="S60" s="37"/>
+      <c r="T60" s="37"/>
+      <c r="U60" s="37"/>
+      <c r="V60" s="37"/>
+      <c r="W60" s="37"/>
+      <c r="X60" s="37"/>
+      <c r="Y60" s="37"/>
+      <c r="Z60" s="37"/>
+      <c r="AA60" s="37"/>
+      <c r="AB60" s="37"/>
+      <c r="AC60" s="37"/>
+      <c r="AD60" s="37"/>
+      <c r="AE60" s="37"/>
+      <c r="AF60" s="37"/>
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A61" s="118"/>
-      <c r="B61" s="118"/>
-      <c r="C61" s="118"/>
-      <c r="D61" s="118"/>
-      <c r="E61" s="118"/>
-      <c r="F61" s="118"/>
-      <c r="G61" s="118"/>
-      <c r="H61" s="118"/>
-      <c r="I61" s="118"/>
-      <c r="J61" s="118"/>
-      <c r="K61" s="118"/>
-      <c r="L61" s="118"/>
-      <c r="M61" s="118"/>
-      <c r="N61" s="118"/>
-      <c r="O61" s="118"/>
-      <c r="P61" s="118"/>
-      <c r="Q61" s="118"/>
-      <c r="R61" s="118"/>
-      <c r="S61" s="118"/>
-      <c r="T61" s="118"/>
-      <c r="U61" s="118"/>
-      <c r="V61" s="118"/>
-      <c r="W61" s="118"/>
-      <c r="X61" s="118"/>
-      <c r="Y61" s="118"/>
-      <c r="Z61" s="118"/>
-      <c r="AA61" s="118"/>
-      <c r="AB61" s="118"/>
-      <c r="AC61" s="118"/>
-      <c r="AD61" s="118"/>
-      <c r="AE61" s="118"/>
-      <c r="AF61" s="118"/>
+      <c r="A61" s="37"/>
+      <c r="B61" s="37"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="37"/>
+      <c r="J61" s="37"/>
+      <c r="K61" s="37"/>
+      <c r="L61" s="37"/>
+      <c r="M61" s="37"/>
+      <c r="N61" s="37"/>
+      <c r="O61" s="37"/>
+      <c r="P61" s="37"/>
+      <c r="Q61" s="37"/>
+      <c r="R61" s="37"/>
+      <c r="S61" s="37"/>
+      <c r="T61" s="37"/>
+      <c r="U61" s="37"/>
+      <c r="V61" s="37"/>
+      <c r="W61" s="37"/>
+      <c r="X61" s="37"/>
+      <c r="Y61" s="37"/>
+      <c r="Z61" s="37"/>
+      <c r="AA61" s="37"/>
+      <c r="AB61" s="37"/>
+      <c r="AC61" s="37"/>
+      <c r="AD61" s="37"/>
+      <c r="AE61" s="37"/>
+      <c r="AF61" s="37"/>
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A62" s="118"/>
-      <c r="B62" s="118"/>
-      <c r="C62" s="118"/>
-      <c r="D62" s="118"/>
-      <c r="E62" s="118"/>
-      <c r="F62" s="118"/>
-      <c r="G62" s="118"/>
-      <c r="H62" s="118"/>
-      <c r="I62" s="118"/>
-      <c r="J62" s="118"/>
-      <c r="K62" s="118"/>
-      <c r="L62" s="118"/>
-      <c r="M62" s="118"/>
-      <c r="N62" s="118"/>
-      <c r="O62" s="118"/>
-      <c r="P62" s="118"/>
-      <c r="Q62" s="118"/>
-      <c r="R62" s="118"/>
-      <c r="S62" s="118"/>
-      <c r="T62" s="118"/>
-      <c r="U62" s="118"/>
-      <c r="V62" s="118"/>
-      <c r="W62" s="118"/>
-      <c r="X62" s="118"/>
-      <c r="Y62" s="118"/>
-      <c r="Z62" s="118"/>
-      <c r="AA62" s="118"/>
-      <c r="AB62" s="118"/>
-      <c r="AC62" s="118"/>
-      <c r="AD62" s="118"/>
-      <c r="AE62" s="118"/>
-      <c r="AF62" s="118"/>
+      <c r="A62" s="37"/>
+      <c r="B62" s="37"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="37"/>
+      <c r="H62" s="37"/>
+      <c r="I62" s="37"/>
+      <c r="J62" s="37"/>
+      <c r="K62" s="37"/>
+      <c r="L62" s="37"/>
+      <c r="M62" s="37"/>
+      <c r="N62" s="37"/>
+      <c r="O62" s="37"/>
+      <c r="P62" s="37"/>
+      <c r="Q62" s="37"/>
+      <c r="R62" s="37"/>
+      <c r="S62" s="37"/>
+      <c r="T62" s="37"/>
+      <c r="U62" s="37"/>
+      <c r="V62" s="37"/>
+      <c r="W62" s="37"/>
+      <c r="X62" s="37"/>
+      <c r="Y62" s="37"/>
+      <c r="Z62" s="37"/>
+      <c r="AA62" s="37"/>
+      <c r="AB62" s="37"/>
+      <c r="AC62" s="37"/>
+      <c r="AD62" s="37"/>
+      <c r="AE62" s="37"/>
+      <c r="AF62" s="37"/>
     </row>
     <row r="63" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A63" s="118"/>
-      <c r="B63" s="118"/>
-      <c r="C63" s="118"/>
-      <c r="D63" s="118"/>
-      <c r="E63" s="118"/>
-      <c r="F63" s="118"/>
-      <c r="G63" s="118"/>
-      <c r="H63" s="118"/>
-      <c r="I63" s="118"/>
-      <c r="J63" s="118"/>
-      <c r="K63" s="118"/>
-      <c r="L63" s="118"/>
-      <c r="M63" s="118"/>
-      <c r="N63" s="118"/>
-      <c r="O63" s="118"/>
-      <c r="P63" s="118"/>
-      <c r="Q63" s="118"/>
-      <c r="R63" s="118"/>
-      <c r="S63" s="118"/>
-      <c r="T63" s="118"/>
-      <c r="U63" s="118"/>
-      <c r="V63" s="118"/>
-      <c r="W63" s="118"/>
-      <c r="X63" s="118"/>
-      <c r="Y63" s="118"/>
-      <c r="Z63" s="118"/>
-      <c r="AA63" s="118"/>
-      <c r="AB63" s="118"/>
-      <c r="AC63" s="118"/>
-      <c r="AD63" s="118"/>
-      <c r="AE63" s="118"/>
-      <c r="AF63" s="118"/>
+      <c r="A63" s="37"/>
+      <c r="B63" s="37"/>
+      <c r="C63" s="37"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
+      <c r="G63" s="37"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="37"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
+      <c r="L63" s="37"/>
+      <c r="M63" s="37"/>
+      <c r="N63" s="37"/>
+      <c r="O63" s="37"/>
+      <c r="P63" s="37"/>
+      <c r="Q63" s="37"/>
+      <c r="R63" s="37"/>
+      <c r="S63" s="37"/>
+      <c r="T63" s="37"/>
+      <c r="U63" s="37"/>
+      <c r="V63" s="37"/>
+      <c r="W63" s="37"/>
+      <c r="X63" s="37"/>
+      <c r="Y63" s="37"/>
+      <c r="Z63" s="37"/>
+      <c r="AA63" s="37"/>
+      <c r="AB63" s="37"/>
+      <c r="AC63" s="37"/>
+      <c r="AD63" s="37"/>
+      <c r="AE63" s="37"/>
+      <c r="AF63" s="37"/>
     </row>
     <row r="64" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A64" s="118"/>
-      <c r="B64" s="118"/>
-      <c r="C64" s="118"/>
-      <c r="D64" s="118"/>
-      <c r="E64" s="118"/>
-      <c r="F64" s="118"/>
-      <c r="G64" s="118"/>
-      <c r="H64" s="118"/>
-      <c r="I64" s="118"/>
-      <c r="J64" s="118"/>
-      <c r="K64" s="118"/>
-      <c r="L64" s="118"/>
-      <c r="M64" s="118"/>
-      <c r="N64" s="118"/>
-      <c r="O64" s="118"/>
-      <c r="P64" s="118"/>
-      <c r="Q64" s="118"/>
-      <c r="R64" s="118"/>
-      <c r="S64" s="118"/>
-      <c r="T64" s="118"/>
-      <c r="U64" s="118"/>
-      <c r="V64" s="118"/>
-      <c r="W64" s="118"/>
-      <c r="X64" s="118"/>
-      <c r="Y64" s="118"/>
-      <c r="Z64" s="118"/>
-      <c r="AA64" s="118"/>
-      <c r="AB64" s="118"/>
-      <c r="AC64" s="118"/>
-      <c r="AD64" s="118"/>
-      <c r="AE64" s="118"/>
-      <c r="AF64" s="118"/>
+      <c r="A64" s="37"/>
+      <c r="B64" s="37"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="37"/>
+      <c r="I64" s="37"/>
+      <c r="J64" s="37"/>
+      <c r="K64" s="37"/>
+      <c r="L64" s="37"/>
+      <c r="M64" s="37"/>
+      <c r="N64" s="37"/>
+      <c r="O64" s="37"/>
+      <c r="P64" s="37"/>
+      <c r="Q64" s="37"/>
+      <c r="R64" s="37"/>
+      <c r="S64" s="37"/>
+      <c r="T64" s="37"/>
+      <c r="U64" s="37"/>
+      <c r="V64" s="37"/>
+      <c r="W64" s="37"/>
+      <c r="X64" s="37"/>
+      <c r="Y64" s="37"/>
+      <c r="Z64" s="37"/>
+      <c r="AA64" s="37"/>
+      <c r="AB64" s="37"/>
+      <c r="AC64" s="37"/>
+      <c r="AD64" s="37"/>
+      <c r="AE64" s="37"/>
+      <c r="AF64" s="37"/>
     </row>
     <row r="65" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A65" s="118"/>
-      <c r="B65" s="118"/>
-      <c r="C65" s="118"/>
-      <c r="D65" s="118"/>
-      <c r="E65" s="118"/>
-      <c r="F65" s="118"/>
-      <c r="G65" s="118"/>
-      <c r="H65" s="118"/>
-      <c r="I65" s="118"/>
-      <c r="J65" s="118"/>
-      <c r="K65" s="118"/>
-      <c r="L65" s="118"/>
-      <c r="M65" s="118"/>
-      <c r="N65" s="118"/>
-      <c r="O65" s="118"/>
-      <c r="P65" s="118"/>
-      <c r="Q65" s="118"/>
-      <c r="R65" s="118"/>
-      <c r="S65" s="118"/>
-      <c r="T65" s="118"/>
-      <c r="U65" s="118"/>
-      <c r="V65" s="118"/>
-      <c r="W65" s="118"/>
-      <c r="X65" s="118"/>
-      <c r="Y65" s="118"/>
-      <c r="Z65" s="118"/>
-      <c r="AA65" s="118"/>
-      <c r="AB65" s="118"/>
-      <c r="AC65" s="118"/>
-      <c r="AD65" s="118"/>
-      <c r="AE65" s="118"/>
-      <c r="AF65" s="118"/>
+      <c r="A65" s="37"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="37"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="37"/>
+      <c r="J65" s="37"/>
+      <c r="K65" s="37"/>
+      <c r="L65" s="37"/>
+      <c r="M65" s="37"/>
+      <c r="N65" s="37"/>
+      <c r="O65" s="37"/>
+      <c r="P65" s="37"/>
+      <c r="Q65" s="37"/>
+      <c r="R65" s="37"/>
+      <c r="S65" s="37"/>
+      <c r="T65" s="37"/>
+      <c r="U65" s="37"/>
+      <c r="V65" s="37"/>
+      <c r="W65" s="37"/>
+      <c r="X65" s="37"/>
+      <c r="Y65" s="37"/>
+      <c r="Z65" s="37"/>
+      <c r="AA65" s="37"/>
+      <c r="AB65" s="37"/>
+      <c r="AC65" s="37"/>
+      <c r="AD65" s="37"/>
+      <c r="AE65" s="37"/>
+      <c r="AF65" s="37"/>
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A66" s="118"/>
-      <c r="B66" s="118"/>
-      <c r="C66" s="118"/>
-      <c r="D66" s="118"/>
-      <c r="E66" s="118"/>
-      <c r="F66" s="118"/>
-      <c r="G66" s="118"/>
-      <c r="H66" s="118"/>
-      <c r="I66" s="118"/>
-      <c r="J66" s="118"/>
-      <c r="K66" s="118"/>
-      <c r="L66" s="118"/>
-      <c r="M66" s="118"/>
-      <c r="N66" s="118"/>
-      <c r="O66" s="118"/>
-      <c r="P66" s="118"/>
-      <c r="Q66" s="118"/>
-      <c r="R66" s="118"/>
-      <c r="S66" s="118"/>
-      <c r="T66" s="118"/>
-      <c r="U66" s="118"/>
-      <c r="V66" s="118"/>
-      <c r="W66" s="118"/>
-      <c r="X66" s="118"/>
-      <c r="Y66" s="118"/>
-      <c r="Z66" s="118"/>
-      <c r="AA66" s="118"/>
-      <c r="AB66" s="118"/>
-      <c r="AC66" s="118"/>
-      <c r="AD66" s="118"/>
-      <c r="AE66" s="118"/>
-      <c r="AF66" s="118"/>
+      <c r="A66" s="37"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="37"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="37"/>
+      <c r="G66" s="37"/>
+      <c r="H66" s="37"/>
+      <c r="I66" s="37"/>
+      <c r="J66" s="37"/>
+      <c r="K66" s="37"/>
+      <c r="L66" s="37"/>
+      <c r="M66" s="37"/>
+      <c r="N66" s="37"/>
+      <c r="O66" s="37"/>
+      <c r="P66" s="37"/>
+      <c r="Q66" s="37"/>
+      <c r="R66" s="37"/>
+      <c r="S66" s="37"/>
+      <c r="T66" s="37"/>
+      <c r="U66" s="37"/>
+      <c r="V66" s="37"/>
+      <c r="W66" s="37"/>
+      <c r="X66" s="37"/>
+      <c r="Y66" s="37"/>
+      <c r="Z66" s="37"/>
+      <c r="AA66" s="37"/>
+      <c r="AB66" s="37"/>
+      <c r="AC66" s="37"/>
+      <c r="AD66" s="37"/>
+      <c r="AE66" s="37"/>
+      <c r="AF66" s="37"/>
     </row>
     <row r="67" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A67" s="118"/>
-      <c r="B67" s="118"/>
-      <c r="C67" s="118"/>
-      <c r="D67" s="118"/>
-      <c r="E67" s="118"/>
-      <c r="F67" s="118"/>
-      <c r="G67" s="118"/>
-      <c r="H67" s="118"/>
-      <c r="I67" s="118"/>
-      <c r="J67" s="118"/>
-      <c r="K67" s="118"/>
-      <c r="L67" s="118"/>
-      <c r="M67" s="118"/>
-      <c r="N67" s="118"/>
-      <c r="O67" s="118"/>
-      <c r="P67" s="118"/>
-      <c r="Q67" s="118"/>
-      <c r="R67" s="118"/>
-      <c r="S67" s="118"/>
-      <c r="T67" s="118"/>
-      <c r="U67" s="118"/>
-      <c r="V67" s="118"/>
-      <c r="W67" s="118"/>
-      <c r="X67" s="118"/>
-      <c r="Y67" s="118"/>
-      <c r="Z67" s="118"/>
-      <c r="AA67" s="118"/>
-      <c r="AB67" s="118"/>
-      <c r="AC67" s="118"/>
-      <c r="AD67" s="118"/>
-      <c r="AE67" s="118"/>
-      <c r="AF67" s="118"/>
+      <c r="A67" s="37"/>
+      <c r="B67" s="37"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="37"/>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="37"/>
+      <c r="J67" s="37"/>
+      <c r="K67" s="37"/>
+      <c r="L67" s="37"/>
+      <c r="M67" s="37"/>
+      <c r="N67" s="37"/>
+      <c r="O67" s="37"/>
+      <c r="P67" s="37"/>
+      <c r="Q67" s="37"/>
+      <c r="R67" s="37"/>
+      <c r="S67" s="37"/>
+      <c r="T67" s="37"/>
+      <c r="U67" s="37"/>
+      <c r="V67" s="37"/>
+      <c r="W67" s="37"/>
+      <c r="X67" s="37"/>
+      <c r="Y67" s="37"/>
+      <c r="Z67" s="37"/>
+      <c r="AA67" s="37"/>
+      <c r="AB67" s="37"/>
+      <c r="AC67" s="37"/>
+      <c r="AD67" s="37"/>
+      <c r="AE67" s="37"/>
+      <c r="AF67" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="Z28:AA28"/>
+    <mergeCell ref="Z29:AA29"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="G2:AC5"/>
+    <mergeCell ref="Y6:AC6"/>
+    <mergeCell ref="AB19:AB23"/>
+    <mergeCell ref="AC19:AC23"/>
+    <mergeCell ref="AA24:AC24"/>
+    <mergeCell ref="H8:N8"/>
+    <mergeCell ref="O27:U27"/>
+    <mergeCell ref="O28:U28"/>
+    <mergeCell ref="O29:U29"/>
+    <mergeCell ref="V28:W28"/>
+    <mergeCell ref="X28:Y28"/>
+    <mergeCell ref="X29:Y29"/>
+    <mergeCell ref="B2:F5"/>
+    <mergeCell ref="H9:N9"/>
+    <mergeCell ref="C25:C44"/>
+    <mergeCell ref="H15:N15"/>
+    <mergeCell ref="H16:N16"/>
+    <mergeCell ref="B25:B44"/>
+    <mergeCell ref="D25:D44"/>
+    <mergeCell ref="E25:E44"/>
+    <mergeCell ref="F25:F44"/>
+    <mergeCell ref="H7:N7"/>
+    <mergeCell ref="H11:N11"/>
+    <mergeCell ref="H12:N12"/>
+    <mergeCell ref="H13:N13"/>
+    <mergeCell ref="H14:N14"/>
+    <mergeCell ref="G41:AA41"/>
+    <mergeCell ref="G42:AA42"/>
+    <mergeCell ref="O6:X6"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="G24:N24"/>
+    <mergeCell ref="H19:N19"/>
+    <mergeCell ref="H20:N20"/>
+    <mergeCell ref="H17:N17"/>
+    <mergeCell ref="H18:N18"/>
+    <mergeCell ref="H21:N21"/>
+    <mergeCell ref="H22:N22"/>
+    <mergeCell ref="H23:N23"/>
+    <mergeCell ref="O19:O23"/>
+    <mergeCell ref="H10:N10"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="G44:AA44"/>
+    <mergeCell ref="Z19:Z23"/>
+    <mergeCell ref="AA19:AA23"/>
+    <mergeCell ref="O33:AA34"/>
+    <mergeCell ref="O35:AA40"/>
+    <mergeCell ref="V26:W26"/>
+    <mergeCell ref="X26:Y26"/>
+    <mergeCell ref="Z26:AA26"/>
+    <mergeCell ref="V27:W27"/>
+    <mergeCell ref="X27:Y27"/>
+    <mergeCell ref="Z27:AA27"/>
+    <mergeCell ref="O30:AA30"/>
+    <mergeCell ref="O25:AA25"/>
+    <mergeCell ref="O31:AA32"/>
+    <mergeCell ref="Y19:Y23"/>
+    <mergeCell ref="O26:U26"/>
     <mergeCell ref="A46:AF67"/>
     <mergeCell ref="B45:AF45"/>
     <mergeCell ref="H6:N6"/>
@@ -5755,66 +5842,6 @@
     <mergeCell ref="U19:U23"/>
     <mergeCell ref="G25:N40"/>
     <mergeCell ref="G43:AA43"/>
-    <mergeCell ref="G44:AA44"/>
-    <mergeCell ref="Z19:Z23"/>
-    <mergeCell ref="AA19:AA23"/>
-    <mergeCell ref="O33:AA34"/>
-    <mergeCell ref="O35:AA40"/>
-    <mergeCell ref="V26:W26"/>
-    <mergeCell ref="X26:Y26"/>
-    <mergeCell ref="Z26:AA26"/>
-    <mergeCell ref="V27:W27"/>
-    <mergeCell ref="X27:Y27"/>
-    <mergeCell ref="Z27:AA27"/>
-    <mergeCell ref="O30:AA30"/>
-    <mergeCell ref="O25:AA25"/>
-    <mergeCell ref="O31:AA32"/>
-    <mergeCell ref="O6:X6"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="G24:N24"/>
-    <mergeCell ref="H19:N19"/>
-    <mergeCell ref="H20:N20"/>
-    <mergeCell ref="H17:N17"/>
-    <mergeCell ref="H18:N18"/>
-    <mergeCell ref="Y19:Y23"/>
-    <mergeCell ref="H21:N21"/>
-    <mergeCell ref="H22:N22"/>
-    <mergeCell ref="H23:N23"/>
-    <mergeCell ref="O19:O23"/>
-    <mergeCell ref="H10:N10"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B2:F5"/>
-    <mergeCell ref="H9:N9"/>
-    <mergeCell ref="C25:C44"/>
-    <mergeCell ref="H15:N15"/>
-    <mergeCell ref="H16:N16"/>
-    <mergeCell ref="B25:B44"/>
-    <mergeCell ref="D25:D44"/>
-    <mergeCell ref="E25:E44"/>
-    <mergeCell ref="F25:F44"/>
-    <mergeCell ref="H7:N7"/>
-    <mergeCell ref="H11:N11"/>
-    <mergeCell ref="H12:N12"/>
-    <mergeCell ref="H13:N13"/>
-    <mergeCell ref="H14:N14"/>
-    <mergeCell ref="G41:AA41"/>
-    <mergeCell ref="G42:AA42"/>
-    <mergeCell ref="O26:U26"/>
-    <mergeCell ref="O27:U27"/>
-    <mergeCell ref="O28:U28"/>
-    <mergeCell ref="O29:U29"/>
-    <mergeCell ref="V28:W28"/>
-    <mergeCell ref="X28:Y28"/>
-    <mergeCell ref="X29:Y29"/>
-    <mergeCell ref="Z28:AA28"/>
-    <mergeCell ref="Z29:AA29"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="G2:AC5"/>
-    <mergeCell ref="Y6:AC6"/>
-    <mergeCell ref="AB19:AB23"/>
-    <mergeCell ref="AC19:AC23"/>
-    <mergeCell ref="AA24:AC24"/>
-    <mergeCell ref="H8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>